<commit_message>
add template and log
</commit_message>
<xml_diff>
--- a/sessions/Mutiple Session Results - 29032022/Session Results (29th March 2022).xlsx
+++ b/sessions/Mutiple Session Results - 29032022/Session Results (29th March 2022).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\sessions\Mutiple Session Results - 29032022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8239673A-10B4-4F50-8173-BC2F6B874102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7869387B-23CC-4852-A36D-63DA2E7B747F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M=1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="11">
   <si>
     <t>Number Of Times Pregnant</t>
   </si>
@@ -449,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R54"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="A1:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,7 +536,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A52" si="0">A4+1</f>
+        <f t="shared" ref="A5:A32" si="0">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -705,160 +705,40 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="6">
-        <f>SUM(B3:B52)/50</f>
-        <v>0</v>
-      </c>
-      <c r="C54" s="6">
-        <f t="shared" ref="C54:I54" si="1">SUM(C3:C52)/50</f>
-        <v>0</v>
-      </c>
-      <c r="D54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I54" s="6">
-        <f t="shared" si="1"/>
+      <c r="B34" s="6">
+        <f>SUM(B3:B32)/30</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="6">
+        <f>SUM(C3:C32)/30</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
+        <f>SUM(D3:D32)/30</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="6">
+        <f>SUM(E3:E32)/30</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="6">
+        <f>SUM(F3:F32)/30</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="6">
+        <f>SUM(G3:G32)/30</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="6">
+        <f>SUM(H3:H32)/30</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="6">
+        <f>SUM(I3:I32)/30</f>
         <v>0</v>
       </c>
     </row>
@@ -1266,406 +1146,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5B8D8A-A482-4E7B-B7BC-223A8E6E8A04}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:I54"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="9" width="18.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <f>A3+1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <f t="shared" ref="A5:A52" si="0">A4+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="6">
-        <f>SUM(B3:B52)/50</f>
-        <v>0</v>
-      </c>
-      <c r="C54" s="6">
-        <f t="shared" ref="C54:I54" si="1">SUM(C3:C52)/50</f>
-        <v>0</v>
-      </c>
-      <c r="D54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAAE03A-A318-41FA-8F05-135F0B79F83E}">
-  <dimension ref="A1:I54"/>
-  <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:I54"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1725,11 +1209,17 @@
         <f>A3+1</f>
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A52" si="0">A4+1</f>
+        <f t="shared" ref="A5:A32" si="0">A4+1</f>
         <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1894,159 +1384,39 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="6">
-        <f>SUM(B3:B52)/50</f>
-        <v>0</v>
-      </c>
-      <c r="C54" s="6">
-        <f t="shared" ref="C54:I54" si="1">SUM(C3:C52)/50</f>
-        <v>0</v>
-      </c>
-      <c r="D54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I54" s="6">
+      <c r="B34" s="6">
+        <f>SUM(B3:B32)/30</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" ref="C34:I34" si="1">SUM(C3:C32)/30</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2056,12 +1426,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E31B93-D821-4DD2-B907-DCA43FD0730B}">
-  <dimension ref="A1:I54"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAAE03A-A318-41FA-8F05-135F0B79F83E}">
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:I54"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2124,7 +1494,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A52" si="0">A4+1</f>
+        <f t="shared" ref="A5:A30" si="0">A4+1</f>
         <v>3</v>
       </c>
     </row>
@@ -2194,255 +1564,123 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="6">
-        <f>SUM(B3:B52)/50</f>
-        <v>0</v>
-      </c>
-      <c r="C54" s="6">
-        <f t="shared" ref="C54:I54" si="1">SUM(C3:C52)/50</f>
-        <v>0</v>
-      </c>
-      <c r="D54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I54" s="6">
+      <c r="B32" s="6">
+        <f>SUM(B3:B30)/30</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" ref="C32:I32" si="1">SUM(C3:C30)/30</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2452,12 +1690,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E593DE3-4F0A-4F22-98BD-01BD8440CE88}">
-  <dimension ref="A1:I54"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E31B93-D821-4DD2-B907-DCA43FD0730B}">
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:I54"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2520,7 +1758,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A52" si="0">A4+1</f>
+        <f t="shared" ref="A5:A32" si="0">A4+1</f>
         <v>3</v>
       </c>
     </row>
@@ -2686,159 +1924,303 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="6">
-        <f>SUM(B3:B52)/50</f>
-        <v>0</v>
-      </c>
-      <c r="C54" s="6">
-        <f t="shared" ref="C54:I54" si="1">SUM(C3:C52)/50</f>
-        <v>0</v>
-      </c>
-      <c r="D54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I54" s="6">
+      <c r="B34" s="6">
+        <f>SUM(B3:B32)/30</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" ref="C34:I34" si="1">SUM(C3:C32)/30</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E593DE3-4F0A-4F22-98BD-01BD8440CE88}">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="9" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <f>A3+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <f t="shared" ref="A5:A30" si="0">A4+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="6">
+        <f>SUM(B3:B30)/30</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" ref="C32:I32" si="1">SUM(C3:C30)/30</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Add runs for M=3, 31 to 100
</commit_message>
<xml_diff>
--- a/sessions/Mutiple Session Results - 29032022/Session Results (29th March 2022).xlsx
+++ b/sessions/Mutiple Session Results - 29032022/Session Results (29th March 2022).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\sessions\Mutiple Session Results - 29032022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADF2DB3-A53A-4E99-8C0D-6723463B3B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD17B26-0C8B-431A-8804-1409B2FF937E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M=1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="11">
   <si>
     <t>Number Of Times Pregnant</t>
   </si>
@@ -3564,7 +3564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5B8D8A-A482-4E7B-B7BC-223A8E6E8A04}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="K97" sqref="K97"/>
     </sheetView>
   </sheetViews>
@@ -6661,8 +6661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAAE03A-A318-41FA-8F05-135F0B79F83E}">
   <dimension ref="A1:I182"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="K99" sqref="K99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7616,35 +7616,59 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
+      <c r="B33" s="7">
+        <v>0.41710000000000003</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0.36959999999999998</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0.2077</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0.41959999999999997</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0.61180000000000001</v>
+      </c>
+      <c r="G33" s="7">
+        <v>2.1105999999999998</v>
+      </c>
+      <c r="H33" s="7">
+        <v>0.85560000000000003</v>
+      </c>
+      <c r="I33" s="7">
+        <v>1.1797</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>1</v>
+      <c r="B34" s="7">
+        <v>0.45689999999999997</v>
+      </c>
+      <c r="C34" s="7">
+        <v>1.0136000000000001</v>
+      </c>
+      <c r="D34" s="7">
+        <v>2.6156999999999999</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0.6996</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0.55020000000000002</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1.4157999999999999</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0.75380000000000003</v>
+      </c>
+      <c r="I34" s="7">
+        <v>1.4834000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -7652,8 +7676,29 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="E35" t="s">
-        <v>1</v>
+      <c r="B35" s="7">
+        <v>0.76910000000000001</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.85470000000000002</v>
+      </c>
+      <c r="D35" s="7">
+        <v>2.4024999999999999</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0.65</v>
+      </c>
+      <c r="F35" s="7">
+        <v>2.7311000000000001</v>
+      </c>
+      <c r="G35" s="7">
+        <v>0.65859999999999996</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0.87529999999999997</v>
+      </c>
+      <c r="I35" s="7">
+        <v>0.89939999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -7661,365 +7706,1829 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
+      <c r="B36" s="7">
+        <v>2.1269</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1.4621999999999999</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1.0301</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0.65539999999999998</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0.74990000000000001</v>
+      </c>
+      <c r="G36" s="7">
+        <v>1.1281000000000001</v>
+      </c>
+      <c r="H36" s="7">
+        <v>1.8906000000000001</v>
+      </c>
+      <c r="I36" s="7">
+        <v>1.5185999999999999</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
+      <c r="B37" s="7">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="C37" s="7">
+        <v>1.2950999999999999</v>
+      </c>
+      <c r="D37" s="7">
+        <v>3.2216999999999998</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0.3609</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0.53369999999999995</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1.3429</v>
+      </c>
+      <c r="H37" s="7">
+        <v>1.5949</v>
+      </c>
+      <c r="I37" s="7">
+        <v>1.1625000000000001</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
+      <c r="B38" s="7">
+        <v>1.3708</v>
+      </c>
+      <c r="C38" s="7">
+        <v>1.0873999999999999</v>
+      </c>
+      <c r="D38" s="7">
+        <v>1.3651</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0.93820000000000003</v>
+      </c>
+      <c r="F38" s="7">
+        <v>1.5282</v>
+      </c>
+      <c r="G38" s="7">
+        <v>1.476</v>
+      </c>
+      <c r="H38" s="7">
+        <v>0.4148</v>
+      </c>
+      <c r="I38" s="7">
+        <v>1.2379</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
+      <c r="B39" s="7">
+        <v>1.0045999999999999</v>
+      </c>
+      <c r="C39" s="7">
+        <v>0.32490000000000002</v>
+      </c>
+      <c r="D39" s="7">
+        <v>3.0596000000000001</v>
+      </c>
+      <c r="E39" s="7">
+        <v>1.5081</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1.2418</v>
+      </c>
+      <c r="G39" s="7">
+        <v>0.89239999999999997</v>
+      </c>
+      <c r="H39" s="7">
+        <v>1.3839999999999999</v>
+      </c>
+      <c r="I39" s="7">
+        <v>1.2798</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
+      <c r="B40" s="7">
+        <v>0.1865</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0.63390000000000002</v>
+      </c>
+      <c r="D40" s="7">
+        <v>3.1099000000000001</v>
+      </c>
+      <c r="E40" s="7">
+        <v>1.6646000000000001</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1.0066999999999999</v>
+      </c>
+      <c r="G40" s="7">
+        <v>1.4599</v>
+      </c>
+      <c r="H40" s="7">
+        <v>1.3976</v>
+      </c>
+      <c r="I40" s="7">
+        <v>1.3108</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
+      <c r="B41" s="7">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="C41" s="7">
+        <v>0.47760000000000002</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0.65680000000000005</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0.79830000000000001</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0.82450000000000001</v>
+      </c>
+      <c r="G41" s="7">
+        <v>1.0112000000000001</v>
+      </c>
+      <c r="H41" s="7">
+        <v>1.2847</v>
+      </c>
+      <c r="I41" s="7">
+        <v>0.87680000000000002</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
+      <c r="B42" s="7">
+        <v>0.95120000000000005</v>
+      </c>
+      <c r="C42" s="7">
+        <v>0.63219999999999998</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0.18579999999999999</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0.75290000000000001</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1.5809</v>
+      </c>
+      <c r="G42" s="7">
+        <v>1.3661000000000001</v>
+      </c>
+      <c r="H42" s="7">
+        <v>1.3446</v>
+      </c>
+      <c r="I42" s="7">
+        <v>1.0246999999999999</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
+      <c r="B43" s="7">
+        <v>1.3058000000000001</v>
+      </c>
+      <c r="C43" s="7">
+        <v>0.72509999999999997</v>
+      </c>
+      <c r="D43" s="7">
+        <v>0.98740000000000006</v>
+      </c>
+      <c r="E43" s="7">
+        <v>1.6411</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0.59819999999999995</v>
+      </c>
+      <c r="G43" s="7">
+        <v>0.84240000000000004</v>
+      </c>
+      <c r="H43" s="7">
+        <v>1.208</v>
+      </c>
+      <c r="I43" s="7">
+        <v>1.0679000000000001</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
+      <c r="B44" s="7">
+        <v>0.1865</v>
+      </c>
+      <c r="C44" s="7">
+        <v>0.77280000000000004</v>
+      </c>
+      <c r="D44" s="7">
+        <v>0.53359999999999996</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0.56289999999999996</v>
+      </c>
+      <c r="F44" s="7">
+        <v>0.54959999999999998</v>
+      </c>
+      <c r="G44" s="7">
+        <v>0.85229999999999995</v>
+      </c>
+      <c r="H44" s="7">
+        <v>0.35570000000000002</v>
+      </c>
+      <c r="I44" s="7">
+        <v>0.47020000000000001</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
+      <c r="B45" s="7">
+        <v>0.91390000000000005</v>
+      </c>
+      <c r="C45" s="7">
+        <v>0.89949999999999997</v>
+      </c>
+      <c r="D45" s="7">
+        <v>2.7648000000000001</v>
+      </c>
+      <c r="E45" s="7">
+        <v>0.71450000000000002</v>
+      </c>
+      <c r="F45" s="7">
+        <v>0.90139999999999998</v>
+      </c>
+      <c r="G45" s="7">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="H45" s="7">
+        <v>2.3203999999999998</v>
+      </c>
+      <c r="I45" s="7">
+        <v>0.82050000000000001</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
+      <c r="B46" s="7">
+        <v>0.83420000000000005</v>
+      </c>
+      <c r="C46" s="7">
+        <v>0.92859999999999998</v>
+      </c>
+      <c r="D46" s="7">
+        <v>1.1337999999999999</v>
+      </c>
+      <c r="E46" s="7">
+        <v>1.0630999999999999</v>
+      </c>
+      <c r="F46" s="7">
+        <v>0.96020000000000005</v>
+      </c>
+      <c r="G46" s="7">
+        <v>1.4970000000000001</v>
+      </c>
+      <c r="H46" s="7">
+        <v>1.3358000000000001</v>
+      </c>
+      <c r="I46" s="7">
+        <v>1.8779999999999999</v>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
+      <c r="B47" s="7">
+        <v>0</v>
+      </c>
+      <c r="C47" s="7">
+        <v>0.46310000000000001</v>
+      </c>
+      <c r="D47" s="7">
+        <v>2.2770999999999999</v>
+      </c>
+      <c r="E47" s="7">
+        <v>0.87609999999999999</v>
+      </c>
+      <c r="F47" s="7">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="G47" s="7">
+        <v>0.4526</v>
+      </c>
+      <c r="H47" s="7">
+        <v>2.2305999999999999</v>
+      </c>
+      <c r="I47" s="7">
+        <v>1.1451</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" s="7">
+        <v>2.3374000000000001</v>
+      </c>
+      <c r="C48" s="7">
+        <v>0.27639999999999998</v>
+      </c>
+      <c r="D48" s="7">
+        <v>2.1242000000000001</v>
+      </c>
+      <c r="E48" s="7">
+        <v>1.6411</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0.4269</v>
+      </c>
+      <c r="G48" s="7">
+        <v>0.52170000000000005</v>
+      </c>
+      <c r="H48" s="7">
+        <v>0.999</v>
+      </c>
+      <c r="I48" s="7">
+        <v>1.0442</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" s="7">
+        <v>1.7198</v>
+      </c>
+      <c r="C49" s="7">
+        <v>0.98809999999999998</v>
+      </c>
+      <c r="D49" s="7">
+        <v>1.8785000000000001</v>
+      </c>
+      <c r="E49" s="7">
+        <v>0.81569999999999998</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0.30449999999999999</v>
+      </c>
+      <c r="G49" s="7">
+        <v>0.59340000000000004</v>
+      </c>
+      <c r="H49" s="7">
+        <v>0.93479999999999996</v>
+      </c>
+      <c r="I49" s="7">
+        <v>1.4884999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" s="7">
+        <v>1.0716000000000001</v>
+      </c>
+      <c r="C50" s="7">
+        <v>1.3672</v>
+      </c>
+      <c r="D50" s="7">
+        <v>1.9550000000000001</v>
+      </c>
+      <c r="E50" s="7">
+        <v>2.1377000000000002</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0.40310000000000001</v>
+      </c>
+      <c r="G50" s="7">
+        <v>0.87070000000000003</v>
+      </c>
+      <c r="H50" s="7">
+        <v>2.0464000000000002</v>
+      </c>
+      <c r="I50" s="7">
+        <v>1.3542000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" s="7">
+        <v>0.76910000000000001</v>
+      </c>
+      <c r="C51" s="7">
+        <v>0.64680000000000004</v>
+      </c>
+      <c r="D51" s="7">
+        <v>3.2866</v>
+      </c>
+      <c r="E51" s="7">
+        <v>1.1052999999999999</v>
+      </c>
+      <c r="F51" s="7">
+        <v>1.0479000000000001</v>
+      </c>
+      <c r="G51" s="7">
+        <v>1.794</v>
+      </c>
+      <c r="H51" s="7">
+        <v>1.7712000000000001</v>
+      </c>
+      <c r="I51" s="7">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" s="7">
+        <v>1.0876999999999999</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0.90759999999999996</v>
+      </c>
+      <c r="D52" s="7">
+        <v>0.39410000000000001</v>
+      </c>
+      <c r="E52" s="7">
+        <v>1.0017</v>
+      </c>
+      <c r="F52" s="7">
+        <v>0.89870000000000005</v>
+      </c>
+      <c r="G52" s="7">
+        <v>0.59619999999999995</v>
+      </c>
+      <c r="H52" s="7">
+        <v>1.9646999999999999</v>
+      </c>
+      <c r="I52" s="7">
+        <v>1.1027</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" s="7">
+        <v>1.1798</v>
+      </c>
+      <c r="C53" s="7">
+        <v>0.72860000000000003</v>
+      </c>
+      <c r="D53" s="7">
+        <v>1.0751999999999999</v>
+      </c>
+      <c r="E53" s="7">
+        <v>1.3660000000000001</v>
+      </c>
+      <c r="F53" s="7">
+        <v>1.0462</v>
+      </c>
+      <c r="G53" s="7">
+        <v>1.7529999999999999</v>
+      </c>
+      <c r="H53" s="7">
+        <v>1.6751</v>
+      </c>
+      <c r="I53" s="7">
+        <v>1.502</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" s="7">
+        <v>1.2514000000000001</v>
+      </c>
+      <c r="C54" s="7">
+        <v>1.7144999999999999</v>
+      </c>
+      <c r="D54" s="7">
+        <v>2.5369999999999999</v>
+      </c>
+      <c r="E54" s="7">
+        <v>1.0157</v>
+      </c>
+      <c r="F54" s="7">
+        <v>0.48149999999999998</v>
+      </c>
+      <c r="G54" s="7">
+        <v>1.1156999999999999</v>
+      </c>
+      <c r="H54" s="7">
+        <v>2.1913999999999998</v>
+      </c>
+      <c r="I54" s="7">
+        <v>0.66869999999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" s="7">
+        <v>0.76910000000000001</v>
+      </c>
+      <c r="C55" s="7">
+        <v>1.0954999999999999</v>
+      </c>
+      <c r="D55" s="7">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="E55" s="7">
+        <v>0.63349999999999995</v>
+      </c>
+      <c r="F55" s="7">
+        <v>1.6342000000000001</v>
+      </c>
+      <c r="G55" s="7">
+        <v>1.107</v>
+      </c>
+      <c r="H55" s="7">
+        <v>0.97119999999999995</v>
+      </c>
+      <c r="I55" s="7">
+        <v>0.75349999999999995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" s="7">
+        <v>1.6047</v>
+      </c>
+      <c r="C56" s="7">
+        <v>1.6284000000000001</v>
+      </c>
+      <c r="D56" s="7">
+        <v>0.50019999999999998</v>
+      </c>
+      <c r="E56" s="7">
+        <v>1.7652000000000001</v>
+      </c>
+      <c r="F56" s="7">
+        <v>0.62560000000000004</v>
+      </c>
+      <c r="G56" s="7">
+        <v>0.64959999999999996</v>
+      </c>
+      <c r="H56" s="7">
+        <v>1.2696000000000001</v>
+      </c>
+      <c r="I56" s="7">
+        <v>0.79249999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" s="7">
+        <v>0.83420000000000005</v>
+      </c>
+      <c r="C57" s="7">
+        <v>1.0448</v>
+      </c>
+      <c r="D57" s="7">
+        <v>2.0308000000000002</v>
+      </c>
+      <c r="E57" s="7">
+        <v>1.6593</v>
+      </c>
+      <c r="F57" s="7">
+        <v>1.1102000000000001</v>
+      </c>
+      <c r="G57" s="7">
+        <v>0.5484</v>
+      </c>
+      <c r="H57" s="7">
+        <v>1.4626999999999999</v>
+      </c>
+      <c r="I57" s="7">
+        <v>1.2216</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" s="7">
+        <v>1.1798</v>
+      </c>
+      <c r="C58" s="7">
+        <v>1.4672000000000001</v>
+      </c>
+      <c r="D58" s="7">
+        <v>1.6301000000000001</v>
+      </c>
+      <c r="E58" s="7">
+        <v>1.1335999999999999</v>
+      </c>
+      <c r="F58" s="7">
+        <v>0.70789999999999997</v>
+      </c>
+      <c r="G58" s="7">
+        <v>0.73319999999999996</v>
+      </c>
+      <c r="H58" s="7">
+        <v>1.1728000000000001</v>
+      </c>
+      <c r="I58" s="7">
+        <v>0.60970000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" s="7">
+        <v>1.7198</v>
+      </c>
+      <c r="C59" s="7">
+        <v>0.76739999999999997</v>
+      </c>
+      <c r="D59" s="7">
+        <v>0.88119999999999998</v>
+      </c>
+      <c r="E59" s="7">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="F59" s="7">
+        <v>0.43330000000000002</v>
+      </c>
+      <c r="G59" s="7">
+        <v>1.0894999999999999</v>
+      </c>
+      <c r="H59" s="7">
+        <v>0.40139999999999998</v>
+      </c>
+      <c r="I59" s="7">
+        <v>1.4123000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" s="7">
+        <v>2.0434999999999999</v>
+      </c>
+      <c r="C60" s="7">
+        <v>1.9692000000000001</v>
+      </c>
+      <c r="D60" s="7">
+        <v>1.1821999999999999</v>
+      </c>
+      <c r="E60" s="7">
+        <v>1.4702999999999999</v>
+      </c>
+      <c r="F60" s="7">
+        <v>0.83809999999999996</v>
+      </c>
+      <c r="G60" s="7">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="H60" s="7">
+        <v>2.4493</v>
+      </c>
+      <c r="I60" s="7">
+        <v>1.2050000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" s="7">
+        <v>1.5829</v>
+      </c>
+      <c r="C61" s="7">
+        <v>1.0914999999999999</v>
+      </c>
+      <c r="D61" s="7">
+        <v>1.7647999999999999</v>
+      </c>
+      <c r="E61" s="7">
+        <v>1.9391</v>
+      </c>
+      <c r="F61" s="7">
+        <v>2.7294999999999998</v>
+      </c>
+      <c r="G61" s="7">
+        <v>0.84379999999999999</v>
+      </c>
+      <c r="H61" s="7">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="I61" s="7">
+        <v>2.4441000000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" s="7">
+        <v>0.55959999999999999</v>
+      </c>
+      <c r="C62" s="7">
+        <v>0.7873</v>
+      </c>
+      <c r="D62" s="7">
+        <v>2.5691000000000002</v>
+      </c>
+      <c r="E62" s="7">
+        <v>0.84960000000000002</v>
+      </c>
+      <c r="F62" s="7">
+        <v>0.87129999999999996</v>
+      </c>
+      <c r="G62" s="7">
+        <v>1.1742999999999999</v>
+      </c>
+      <c r="H62" s="7">
+        <v>1.3712</v>
+      </c>
+      <c r="I62" s="7">
+        <v>1.7790999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" s="7">
+        <v>1.3581000000000001</v>
+      </c>
+      <c r="C63" s="7">
+        <v>1.6156999999999999</v>
+      </c>
+      <c r="D63" s="7">
+        <v>0.70740000000000003</v>
+      </c>
+      <c r="E63" s="7">
+        <v>1.0035000000000001</v>
+      </c>
+      <c r="F63" s="7">
+        <v>0.93269999999999997</v>
+      </c>
+      <c r="G63" s="7">
+        <v>1.234</v>
+      </c>
+      <c r="H63" s="7">
+        <v>1.5166999999999999</v>
+      </c>
+      <c r="I63" s="7">
+        <v>0.82050000000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" s="7">
+        <v>1.3190999999999999</v>
+      </c>
+      <c r="C64" s="7">
+        <v>1.7423999999999999</v>
+      </c>
+      <c r="D64" s="7">
+        <v>0.62309999999999999</v>
+      </c>
+      <c r="E64" s="7">
+        <v>1.1778</v>
+      </c>
+      <c r="F64" s="7">
+        <v>0.36659999999999998</v>
+      </c>
+      <c r="G64" s="7">
+        <v>0.94730000000000003</v>
+      </c>
+      <c r="H64" s="7">
+        <v>0.87629999999999997</v>
+      </c>
+      <c r="I64" s="7">
+        <v>1.6426000000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" s="7">
+        <v>0.95120000000000005</v>
+      </c>
+      <c r="C65" s="7">
+        <v>1.0619000000000001</v>
+      </c>
+      <c r="D65" s="7">
+        <v>2.7223000000000002</v>
+      </c>
+      <c r="E65" s="7">
+        <v>0.99819999999999998</v>
+      </c>
+      <c r="F65" s="7">
+        <v>0.49759999999999999</v>
+      </c>
+      <c r="G65" s="7">
+        <v>0.97140000000000004</v>
+      </c>
+      <c r="H65" s="7">
+        <v>1.2455000000000001</v>
+      </c>
+      <c r="I65" s="7">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" s="7">
+        <v>0.67259999999999998</v>
+      </c>
+      <c r="C66" s="7">
+        <v>0.96140000000000003</v>
+      </c>
+      <c r="D66" s="7">
+        <v>0.68259999999999998</v>
+      </c>
+      <c r="E66" s="7">
+        <v>0.80049999999999999</v>
+      </c>
+      <c r="F66" s="7">
+        <v>0.47039999999999998</v>
+      </c>
+      <c r="G66" s="7">
+        <v>0.73240000000000005</v>
+      </c>
+      <c r="H66" s="7">
+        <v>0.53849999999999998</v>
+      </c>
+      <c r="I66" s="7">
+        <v>1.8874</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" s="7">
+        <v>0.55959999999999999</v>
+      </c>
+      <c r="C67" s="7">
+        <v>0.57889999999999997</v>
+      </c>
+      <c r="D67" s="7">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="E67" s="7">
+        <v>1.1520999999999999</v>
+      </c>
+      <c r="F67" s="7">
+        <v>0.64649999999999996</v>
+      </c>
+      <c r="G67" s="7">
+        <v>0.77410000000000001</v>
+      </c>
+      <c r="H67" s="7">
+        <v>2.5874999999999999</v>
+      </c>
+      <c r="I67" s="7">
+        <v>1.1072</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" s="7">
+        <v>1.3581000000000001</v>
+      </c>
+      <c r="C68" s="7">
+        <v>0.627</v>
+      </c>
+      <c r="D68" s="7">
+        <v>3.3555000000000001</v>
+      </c>
+      <c r="E68" s="7">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="F68" s="7">
+        <v>0.4481</v>
+      </c>
+      <c r="G68" s="7">
+        <v>1.4128000000000001</v>
+      </c>
+      <c r="H68" s="7">
+        <v>0.70289999999999997</v>
+      </c>
+      <c r="I68" s="7">
+        <v>1.4352</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <f t="shared" ref="A69:A102" si="1">A68+1</f>
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" s="7">
+        <v>1.8561000000000001</v>
+      </c>
+      <c r="C69" s="7">
+        <v>0.68389999999999995</v>
+      </c>
+      <c r="D69" s="7">
+        <v>0.65680000000000005</v>
+      </c>
+      <c r="E69" s="7">
+        <v>1.2918000000000001</v>
+      </c>
+      <c r="F69" s="7">
+        <v>1.4979</v>
+      </c>
+      <c r="G69" s="7">
+        <v>0.62539999999999996</v>
+      </c>
+      <c r="H69" s="7">
+        <v>1.7097</v>
+      </c>
+      <c r="I69" s="7">
+        <v>0.86809999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" s="7">
+        <v>1.2652000000000001</v>
+      </c>
+      <c r="C70" s="7">
+        <v>2.1785000000000001</v>
+      </c>
+      <c r="D70" s="7">
+        <v>0.70130000000000003</v>
+      </c>
+      <c r="E70" s="7">
+        <v>1.1762999999999999</v>
+      </c>
+      <c r="F70" s="7">
+        <v>1.2059</v>
+      </c>
+      <c r="G70" s="7">
+        <v>0.47360000000000002</v>
+      </c>
+      <c r="H70" s="7">
+        <v>1.2311000000000001</v>
+      </c>
+      <c r="I70" s="7">
+        <v>1.3979999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" s="7">
+        <v>1.1798</v>
+      </c>
+      <c r="C71" s="7">
+        <v>1.6938</v>
+      </c>
+      <c r="D71" s="7">
+        <v>3.4014000000000002</v>
+      </c>
+      <c r="E71" s="7">
+        <v>0.68689999999999996</v>
+      </c>
+      <c r="F71" s="7">
+        <v>1.4145000000000001</v>
+      </c>
+      <c r="G71" s="7">
+        <v>0.81340000000000001</v>
+      </c>
+      <c r="H71" s="7">
+        <v>0.52459999999999996</v>
+      </c>
+      <c r="I71" s="7">
+        <v>1.8333999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" s="7">
+        <v>1.0045999999999999</v>
+      </c>
+      <c r="C72" s="7">
+        <v>1.0729</v>
+      </c>
+      <c r="D72" s="7">
+        <v>0.9335</v>
+      </c>
+      <c r="E72" s="7">
+        <v>0.47839999999999999</v>
+      </c>
+      <c r="F72" s="7">
+        <v>0.61419999999999997</v>
+      </c>
+      <c r="G72" s="7">
+        <v>0.82520000000000004</v>
+      </c>
+      <c r="H72" s="7">
+        <v>3.1135000000000002</v>
+      </c>
+      <c r="I72" s="7">
+        <v>1.2257</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" s="7">
+        <v>1.3322000000000001</v>
+      </c>
+      <c r="C73" s="7">
+        <v>1.0490999999999999</v>
+      </c>
+      <c r="D73" s="7">
+        <v>3.0141</v>
+      </c>
+      <c r="E73" s="7">
+        <v>1.5921000000000001</v>
+      </c>
+      <c r="F73" s="7">
+        <v>0.23710000000000001</v>
+      </c>
+      <c r="G73" s="7">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="H73" s="7">
+        <v>2.2282000000000002</v>
+      </c>
+      <c r="I73" s="7">
+        <v>1.5992</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" s="7">
+        <v>1.6047</v>
+      </c>
+      <c r="C74" s="7">
+        <v>1.1660999999999999</v>
+      </c>
+      <c r="D74" s="7">
+        <v>2.5148000000000001</v>
+      </c>
+      <c r="E74" s="7">
+        <v>1.1581999999999999</v>
+      </c>
+      <c r="F74" s="7">
+        <v>1.5105999999999999</v>
+      </c>
+      <c r="G74" s="7">
+        <v>0.62190000000000001</v>
+      </c>
+      <c r="H74" s="7">
+        <v>2.8292999999999999</v>
+      </c>
+      <c r="I74" s="7">
+        <v>0.87680000000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" s="7">
+        <v>0.55959999999999999</v>
+      </c>
+      <c r="C75" s="7">
+        <v>1.7528999999999999</v>
+      </c>
+      <c r="D75" s="7">
+        <v>0.91479999999999995</v>
+      </c>
+      <c r="E75" s="7">
+        <v>1.2175</v>
+      </c>
+      <c r="F75" s="7">
+        <v>1.2229000000000001</v>
+      </c>
+      <c r="G75" s="7">
+        <v>2.0543</v>
+      </c>
+      <c r="H75" s="7">
+        <v>1.415</v>
+      </c>
+      <c r="I75" s="7">
+        <v>0.9022</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" s="7">
+        <v>0.1865</v>
+      </c>
+      <c r="C76" s="7">
+        <v>0.51639999999999997</v>
+      </c>
+      <c r="D76" s="7">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="E76" s="7">
+        <v>1.0664</v>
+      </c>
+      <c r="F76" s="7">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="G76" s="7">
+        <v>0.87019999999999997</v>
+      </c>
+      <c r="H76" s="7">
+        <v>0.88719999999999999</v>
+      </c>
+      <c r="I76" s="7">
+        <v>1.5103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" s="7">
+        <v>0.37309999999999999</v>
+      </c>
+      <c r="C77" s="7">
+        <v>1.6302000000000001</v>
+      </c>
+      <c r="D77" s="7">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="E77" s="7">
+        <v>1.0310999999999999</v>
+      </c>
+      <c r="F77" s="7">
+        <v>0.77380000000000004</v>
+      </c>
+      <c r="G77" s="7">
+        <v>0.53290000000000004</v>
+      </c>
+      <c r="H77" s="7">
+        <v>1.0782</v>
+      </c>
+      <c r="I77" s="7">
+        <v>1.3261000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" s="7">
+        <v>1.4688000000000001</v>
+      </c>
+      <c r="C78" s="7">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="D78" s="7">
+        <v>0.91010000000000002</v>
+      </c>
+      <c r="E78" s="7">
+        <v>1.2346999999999999</v>
+      </c>
+      <c r="F78" s="7">
+        <v>0.37819999999999998</v>
+      </c>
+      <c r="G78" s="7">
+        <v>0.81950000000000001</v>
+      </c>
+      <c r="H78" s="7">
+        <v>1.2934000000000001</v>
+      </c>
+      <c r="I78" s="7">
+        <v>1.3261000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" s="7">
+        <v>1.1944999999999999</v>
+      </c>
+      <c r="C79" s="7">
+        <v>0.93210000000000004</v>
+      </c>
+      <c r="D79" s="7">
+        <v>2.7818999999999998</v>
+      </c>
+      <c r="E79" s="7">
+        <v>0.99460000000000004</v>
+      </c>
+      <c r="F79" s="7">
+        <v>0.872</v>
+      </c>
+      <c r="G79" s="7">
+        <v>0.9657</v>
+      </c>
+      <c r="H79" s="7">
+        <v>1.6636</v>
+      </c>
+      <c r="I79" s="7">
+        <v>1.3299000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" s="7">
+        <v>1.7598</v>
+      </c>
+      <c r="C80" s="7">
+        <v>1.0605</v>
+      </c>
+      <c r="D80" s="7">
+        <v>2.5215999999999998</v>
+      </c>
+      <c r="E80" s="7">
+        <v>0.34089999999999998</v>
+      </c>
+      <c r="F80" s="7">
+        <v>0.59719999999999995</v>
+      </c>
+      <c r="G80" s="7">
+        <v>2.1328</v>
+      </c>
+      <c r="H80" s="7">
+        <v>1.0839000000000001</v>
+      </c>
+      <c r="I80" s="7">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" s="7">
+        <v>0.61870000000000003</v>
+      </c>
+      <c r="C81" s="7">
+        <v>0.94920000000000004</v>
+      </c>
+      <c r="D81" s="7">
+        <v>0.84109999999999996</v>
+      </c>
+      <c r="E81" s="7">
+        <v>1.2712000000000001</v>
+      </c>
+      <c r="F81" s="7">
+        <v>0.90629999999999999</v>
+      </c>
+      <c r="G81" s="7">
+        <v>1.4944</v>
+      </c>
+      <c r="H81" s="7">
+        <v>1.7796000000000001</v>
+      </c>
+      <c r="I81" s="7">
+        <v>1.8044</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" s="7">
+        <v>1.5383</v>
+      </c>
+      <c r="C82" s="7">
+        <v>1.2547999999999999</v>
+      </c>
+      <c r="D82" s="7">
+        <v>2.9211</v>
+      </c>
+      <c r="E82" s="7">
+        <v>0.46339999999999998</v>
+      </c>
+      <c r="F82" s="7">
+        <v>0.7611</v>
+      </c>
+      <c r="G82" s="7">
+        <v>1.4027000000000001</v>
+      </c>
+      <c r="H82" s="7">
+        <v>1.7923</v>
+      </c>
+      <c r="I82" s="7">
+        <v>1.4646999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" s="7">
+        <v>2.5097</v>
+      </c>
+      <c r="C83" s="7">
+        <v>0.65180000000000005</v>
+      </c>
+      <c r="D83" s="7">
+        <v>2.3898999999999999</v>
+      </c>
+      <c r="E83" s="7">
+        <v>1.2303999999999999</v>
+      </c>
+      <c r="F83" s="7">
+        <v>0.84430000000000005</v>
+      </c>
+      <c r="G83" s="7">
+        <v>1.1209</v>
+      </c>
+      <c r="H83" s="7">
+        <v>1.3695999999999999</v>
+      </c>
+      <c r="I83" s="7">
+        <v>1.264</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" s="7">
+        <v>0.67259999999999998</v>
+      </c>
+      <c r="C84" s="7">
+        <v>0.65620000000000001</v>
+      </c>
+      <c r="D84" s="7">
+        <v>0.52539999999999998</v>
+      </c>
+      <c r="E84" s="7">
+        <v>0.80920000000000003</v>
+      </c>
+      <c r="F84" s="7">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="G84" s="7">
+        <v>1.2827999999999999</v>
+      </c>
+      <c r="H84" s="7">
+        <v>1.4578</v>
+      </c>
+      <c r="I84" s="7">
+        <v>1.1094999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" s="7">
+        <v>1.7499</v>
+      </c>
+      <c r="C85" s="7">
+        <v>0.62009999999999998</v>
+      </c>
+      <c r="D85" s="7">
+        <v>0.66979999999999995</v>
+      </c>
+      <c r="E85" s="7">
+        <v>0.87609999999999999</v>
+      </c>
+      <c r="F85" s="7">
+        <v>0.5968</v>
+      </c>
+      <c r="G85" s="7">
+        <v>0.86229999999999996</v>
+      </c>
+      <c r="H85" s="7">
+        <v>1.7802</v>
+      </c>
+      <c r="I85" s="7">
+        <v>1.0934999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" s="7">
+        <v>1.7299</v>
+      </c>
+      <c r="C86" s="7">
+        <v>1.4162999999999999</v>
+      </c>
+      <c r="D86" s="7">
+        <v>2.0749</v>
+      </c>
+      <c r="E86" s="7">
+        <v>0.79610000000000003</v>
+      </c>
+      <c r="F86" s="7">
+        <v>0.39539999999999997</v>
+      </c>
+      <c r="G86" s="7">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="H86" s="7">
+        <v>1.2742</v>
+      </c>
+      <c r="I86" s="7">
+        <v>1.7478</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" s="7">
+        <v>0.83420000000000005</v>
+      </c>
+      <c r="C87" s="7">
+        <v>1.2222</v>
+      </c>
+      <c r="D87" s="7">
+        <v>1.1489</v>
+      </c>
+      <c r="E87" s="7">
+        <v>1.3387</v>
+      </c>
+      <c r="F87" s="7">
+        <v>0.59309999999999996</v>
+      </c>
+      <c r="G87" s="7">
+        <v>0.52659999999999996</v>
+      </c>
+      <c r="H87" s="7">
+        <v>1.6295999999999999</v>
+      </c>
+      <c r="I87" s="7">
+        <v>1.075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88" s="7">
+        <v>1.3452</v>
+      </c>
+      <c r="C88" s="7">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="D88" s="7">
+        <v>1.3808</v>
+      </c>
+      <c r="E88" s="7">
+        <v>1.4739</v>
+      </c>
+      <c r="F88" s="7">
+        <v>0.82730000000000004</v>
+      </c>
+      <c r="G88" s="7">
+        <v>1.3527</v>
+      </c>
+      <c r="H88" s="7">
+        <v>1.4525999999999999</v>
+      </c>
+      <c r="I88" s="7">
+        <v>0.64959999999999996</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" s="7">
+        <v>1.8561000000000001</v>
+      </c>
+      <c r="C89" s="7">
+        <v>1.2708999999999999</v>
+      </c>
+      <c r="D89" s="7">
+        <v>0.74890000000000001</v>
+      </c>
+      <c r="E89" s="7">
+        <v>1.1005</v>
+      </c>
+      <c r="F89" s="7">
+        <v>0.27689999999999998</v>
+      </c>
+      <c r="G89" s="7">
+        <v>0.6079</v>
+      </c>
+      <c r="H89" s="7">
+        <v>0.74580000000000002</v>
+      </c>
+      <c r="I89" s="7">
+        <v>0.88249999999999995</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" s="7">
+        <v>2.2694000000000001</v>
+      </c>
+      <c r="C90" s="7">
+        <v>1.0707</v>
+      </c>
+      <c r="D90" s="7">
+        <v>1.1337999999999999</v>
+      </c>
+      <c r="E90" s="7">
+        <v>0.73150000000000004</v>
+      </c>
+      <c r="F90" s="7">
+        <v>1.4594</v>
+      </c>
+      <c r="G90" s="7">
+        <v>1.3502000000000001</v>
+      </c>
+      <c r="H90" s="7">
+        <v>0.91190000000000004</v>
+      </c>
+      <c r="I90" s="7">
+        <v>0.98470000000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" s="7">
+        <v>0.26379999999999998</v>
+      </c>
+      <c r="C91" s="7">
+        <v>0.49869999999999998</v>
+      </c>
+      <c r="D91" s="7">
+        <v>2.2713999999999999</v>
+      </c>
+      <c r="E91" s="7">
+        <v>0.8881</v>
+      </c>
+      <c r="F91" s="7">
+        <v>0.95540000000000003</v>
+      </c>
+      <c r="G91" s="7">
+        <v>0.34939999999999999</v>
+      </c>
+      <c r="H91" s="7">
+        <v>1.97</v>
+      </c>
+      <c r="I91" s="7">
+        <v>1.244</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" s="7">
+        <v>1.4688000000000001</v>
+      </c>
+      <c r="C92" s="7">
+        <v>0.58509999999999995</v>
+      </c>
+      <c r="D92" s="7">
+        <v>1.4891000000000001</v>
+      </c>
+      <c r="E92" s="7">
+        <v>0.92110000000000003</v>
+      </c>
+      <c r="F92" s="7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G92" s="7">
+        <v>1.0617000000000001</v>
+      </c>
+      <c r="H92" s="7">
+        <v>1.8688</v>
+      </c>
+      <c r="I92" s="7">
+        <v>0.45939999999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" s="7">
+        <v>1.4207000000000001</v>
+      </c>
+      <c r="C93" s="7">
+        <v>0.26440000000000002</v>
+      </c>
+      <c r="D93" s="7">
+        <v>1.0671999999999999</v>
+      </c>
+      <c r="E93" s="7">
+        <v>1.6782999999999999</v>
+      </c>
+      <c r="F93" s="7">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="G93" s="7">
+        <v>0.76170000000000004</v>
+      </c>
+      <c r="H93" s="7">
+        <v>0.6452</v>
+      </c>
+      <c r="I93" s="7">
+        <v>0.77649999999999997</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" s="7">
+        <v>0.55959999999999999</v>
+      </c>
+      <c r="C94" s="7">
+        <v>0.85089999999999999</v>
+      </c>
+      <c r="D94" s="7">
+        <v>0.92889999999999995</v>
+      </c>
+      <c r="E94" s="7">
+        <v>0.46339999999999998</v>
+      </c>
+      <c r="F94" s="7">
+        <v>0.25979999999999998</v>
+      </c>
+      <c r="G94" s="7">
+        <v>1.1001000000000001</v>
+      </c>
+      <c r="H94" s="7">
+        <v>2.1648999999999998</v>
+      </c>
+      <c r="I94" s="7">
+        <v>0.77969999999999995</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" s="7">
+        <v>1.3190999999999999</v>
+      </c>
+      <c r="C95" s="7">
+        <v>1.0887</v>
+      </c>
+      <c r="D95" s="7">
+        <v>0.34749999999999998</v>
+      </c>
+      <c r="E95" s="7">
+        <v>0.68689999999999996</v>
+      </c>
+      <c r="F95" s="7">
+        <v>0.22239999999999999</v>
+      </c>
+      <c r="G95" s="7">
+        <v>1.0335000000000001</v>
+      </c>
+      <c r="H95" s="7">
+        <v>1.8574999999999999</v>
+      </c>
+      <c r="I95" s="7">
+        <v>1.1516999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <f t="shared" si="1"/>
         <v>94</v>
+      </c>
+      <c r="B96" s="7">
+        <v>1.8839999999999999</v>
+      </c>
+      <c r="C96" s="7">
+        <v>1.2057</v>
+      </c>
+      <c r="D96" s="7">
+        <v>1.1564000000000001</v>
+      </c>
+      <c r="E96" s="7">
+        <v>1.1897</v>
+      </c>
+      <c r="F96" s="7">
+        <v>0.87439999999999996</v>
+      </c>
+      <c r="G96" s="7">
+        <v>1.1428</v>
+      </c>
+      <c r="H96" s="7">
+        <v>0.23080000000000001</v>
+      </c>
+      <c r="I96" s="7">
+        <v>0.8881</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -8027,35 +9536,179 @@
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
+      <c r="B97" s="7">
+        <v>1.9830000000000001</v>
+      </c>
+      <c r="C97" s="7">
+        <v>1.1572</v>
+      </c>
+      <c r="D97" s="7">
+        <v>0.67620000000000002</v>
+      </c>
+      <c r="E97" s="7">
+        <v>1.2073</v>
+      </c>
+      <c r="F97" s="7">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="G97" s="7">
+        <v>1.2847</v>
+      </c>
+      <c r="H97" s="7">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="I97" s="7">
+        <v>1.1027</v>
+      </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
+      <c r="B98" s="7">
+        <v>1.1193</v>
+      </c>
+      <c r="C98" s="7">
+        <v>0.75509999999999999</v>
+      </c>
+      <c r="D98" s="7">
+        <v>2.0137</v>
+      </c>
+      <c r="E98" s="7">
+        <v>1.0697000000000001</v>
+      </c>
+      <c r="F98" s="7">
+        <v>2.5207000000000002</v>
+      </c>
+      <c r="G98" s="7">
+        <v>1.3055000000000001</v>
+      </c>
+      <c r="H98" s="7">
+        <v>1.3299000000000001</v>
+      </c>
+      <c r="I98" s="7">
+        <v>0.90769999999999995</v>
+      </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
+      <c r="B99" s="7">
+        <v>2.7980999999999998</v>
+      </c>
+      <c r="C99" s="7">
+        <v>1.4873000000000001</v>
+      </c>
+      <c r="D99" s="7">
+        <v>2.8081</v>
+      </c>
+      <c r="E99" s="7">
+        <v>1.5439000000000001</v>
+      </c>
+      <c r="F99" s="7">
+        <v>0.82089999999999996</v>
+      </c>
+      <c r="G99" s="7">
+        <v>1.1926000000000001</v>
+      </c>
+      <c r="H99" s="7">
+        <v>0.91749999999999998</v>
+      </c>
+      <c r="I99" s="7">
+        <v>1.0911999999999999</v>
+      </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
+      <c r="B100" s="7">
+        <v>1.3322000000000001</v>
+      </c>
+      <c r="C100" s="7">
+        <v>0.62929999999999997</v>
+      </c>
+      <c r="D100" s="7">
+        <v>1.8507</v>
+      </c>
+      <c r="E100" s="7">
+        <v>1.3633999999999999</v>
+      </c>
+      <c r="F100" s="7">
+        <v>1.6528</v>
+      </c>
+      <c r="G100" s="7">
+        <v>0.61470000000000002</v>
+      </c>
+      <c r="H100" s="7">
+        <v>1.9524999999999999</v>
+      </c>
+      <c r="I100" s="7">
+        <v>1.2379</v>
+      </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
+      <c r="B101" s="7">
+        <v>1.3581000000000001</v>
+      </c>
+      <c r="C101" s="7">
+        <v>1.7122999999999999</v>
+      </c>
+      <c r="D101" s="7">
+        <v>0.63</v>
+      </c>
+      <c r="E101" s="7">
+        <v>1.2073</v>
+      </c>
+      <c r="F101" s="7">
+        <v>0.93330000000000002</v>
+      </c>
+      <c r="G101" s="7">
+        <v>1.0631999999999999</v>
+      </c>
+      <c r="H101" s="7">
+        <v>1.0112000000000001</v>
+      </c>
+      <c r="I101" s="7">
+        <v>0.98729999999999996</v>
+      </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
+      </c>
+      <c r="B102" s="7">
+        <v>1.3322000000000001</v>
+      </c>
+      <c r="C102" s="7">
+        <v>1.3028</v>
+      </c>
+      <c r="D102" s="7">
+        <v>2.7080000000000002</v>
+      </c>
+      <c r="E102" s="7">
+        <v>0.79159999999999997</v>
+      </c>
+      <c r="F102" s="7">
+        <v>0.58989999999999998</v>
+      </c>
+      <c r="G102" s="7">
+        <v>1.2381</v>
+      </c>
+      <c r="H102" s="7">
+        <v>0.74519999999999997</v>
+      </c>
+      <c r="I102" s="7">
+        <v>1.1881999999999999</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
@@ -8067,35 +9720,35 @@
       </c>
       <c r="B104" s="6">
         <f>SUM(B3:B102)/100</f>
-        <v>0.28512300000000007</v>
+        <v>1.1229550000000004</v>
       </c>
       <c r="C104" s="6">
         <f t="shared" ref="C104:I104" si="2">SUM(C3:C102)/100</f>
-        <v>0.27922799999999998</v>
+        <v>0.98664499999999999</v>
       </c>
       <c r="D104" s="6">
         <f t="shared" si="2"/>
-        <v>0.48032600000000003</v>
+        <v>1.5775019999999997</v>
       </c>
       <c r="E104" s="6">
         <f t="shared" si="2"/>
-        <v>0.326546</v>
+        <v>1.0653039999999994</v>
       </c>
       <c r="F104" s="6">
         <f t="shared" si="2"/>
-        <v>0.22997400000000007</v>
+        <v>0.8315849999999998</v>
       </c>
       <c r="G104" s="6">
         <f t="shared" si="2"/>
-        <v>0.36247400000000007</v>
+        <v>1.0772819999999999</v>
       </c>
       <c r="H104" s="6">
         <f t="shared" si="2"/>
-        <v>0.31554700000000002</v>
+        <v>1.2884110000000002</v>
       </c>
       <c r="I104" s="6">
         <f t="shared" si="2"/>
-        <v>0.34911700000000001</v>
+        <v>1.174639</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add m=4, 1-100 runs
</commit_message>
<xml_diff>
--- a/sessions/Mutiple Session Results - 29032022/Session Results (29th March 2022).xlsx
+++ b/sessions/Mutiple Session Results - 29032022/Session Results (29th March 2022).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\sessions\Mutiple Session Results - 29032022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD17B26-0C8B-431A-8804-1409B2FF937E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D8BCF5-F820-45B2-ADD0-D93D2CEF4E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M=1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="11">
   <si>
     <t>Number Of Times Pregnant</t>
   </si>
@@ -6661,7 +6661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAAE03A-A318-41FA-8F05-135F0B79F83E}">
   <dimension ref="A1:I182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="K99" sqref="K99"/>
     </sheetView>
   </sheetViews>
@@ -9993,10 +9993,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E31B93-D821-4DD2-B907-DCA43FD0730B}">
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10004,7 +10004,7 @@
     <col min="1" max="9" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -10033,7 +10033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -10046,671 +10046,3156 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="7">
+        <v>0.45689999999999997</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.58289999999999997</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2.3161</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1.5424</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.58230000000000004</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.58189999999999997</v>
+      </c>
+      <c r="H3" s="7">
+        <v>2.3180999999999998</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1.0454000000000001</v>
+      </c>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f>A3+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="7">
+        <v>1.1193</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.9143</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1.7825</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1.1715</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.72</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1.2385999999999999</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1.4382999999999999</v>
+      </c>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" ref="A5:A68" si="0">A4+1</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="7">
+        <v>1.1309</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1.4458</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2.7088000000000001</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.90469999999999995</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.79190000000000005</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.68289999999999995</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.35720000000000002</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.92279999999999995</v>
+      </c>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="7">
+        <v>1.3322000000000001</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.67849999999999999</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1.7734000000000001</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.65810000000000002</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1.4877</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.90480000000000005</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1.3137000000000001</v>
+      </c>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
+        <v>0.36120000000000002</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.73709999999999998</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1.5536000000000001</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1.1684000000000001</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.74760000000000004</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1.0969</v>
+      </c>
+      <c r="H7" s="7">
+        <v>2.3227000000000002</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.76919999999999999</v>
+      </c>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <v>1.3025</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.69189999999999996</v>
+      </c>
+      <c r="D8" s="7">
+        <v>2.9937</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1.5670999999999999</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.74519999999999997</v>
+      </c>
+      <c r="G8" s="7">
+        <v>2.5882999999999998</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1.5817000000000001</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0.83489999999999998</v>
+      </c>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="7">
+        <v>0.51090000000000002</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1.3692</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1.0364</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1.216</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.84650000000000003</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0.88819999999999999</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1.7410000000000001</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1.6811</v>
+      </c>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
+        <v>2.2961</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1.0562</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2.2248999999999999</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.69130000000000003</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2.4258000000000002</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1.0273000000000001</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="I10" s="7">
+        <v>1.6345000000000001</v>
+      </c>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
+        <v>0.48470000000000002</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.81240000000000001</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1.5743</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1.2764</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.45250000000000001</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1.0427</v>
+      </c>
+      <c r="H11" s="7">
+        <v>2.0326</v>
+      </c>
+      <c r="I11" s="7">
+        <v>1.0235000000000001</v>
+      </c>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="7">
+        <v>1.5911</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1.1247</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2.4491999999999998</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1.1718</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.37690000000000001</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1.2819</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0.45960000000000001</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0.70530000000000004</v>
+      </c>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="7">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1.6043000000000001</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1.7861</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1.1660999999999999</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2.2501000000000002</v>
+      </c>
+      <c r="G13" s="7">
+        <v>1.3528</v>
+      </c>
+      <c r="H13" s="7">
+        <v>1.7962</v>
+      </c>
+      <c r="I13" s="7">
+        <v>1.2292000000000001</v>
+      </c>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="7">
+        <v>1.5326</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.79310000000000003</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2.7183999999999999</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.80269999999999997</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1.3364</v>
+      </c>
+      <c r="G14" s="7">
+        <v>2.2513999999999998</v>
+      </c>
+      <c r="H14" s="7">
+        <v>1.3392999999999999</v>
+      </c>
+      <c r="I14" s="7">
+        <v>0.97060000000000002</v>
+      </c>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="7">
+        <v>0.22850000000000001</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.61360000000000003</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1.9981</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1.4937</v>
+      </c>
+      <c r="F15" s="7">
+        <v>2.2223999999999999</v>
+      </c>
+      <c r="G15" s="7">
+        <v>1.4420999999999999</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0.89229999999999998</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" s="7">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1.4729000000000001</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0.56879999999999997</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.7742</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.7974</v>
+      </c>
+      <c r="G16" s="7">
+        <v>2.1349</v>
+      </c>
+      <c r="H16" s="7">
+        <v>1.1668000000000001</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0.89590000000000003</v>
+      </c>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="7">
+        <v>2.1734</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.71550000000000002</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0.82430000000000003</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1.0692999999999999</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="G17" s="7">
+        <v>1.0236000000000001</v>
+      </c>
+      <c r="H17" s="7">
+        <v>1.9865999999999999</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0.83720000000000006</v>
+      </c>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" s="7">
+        <v>0.36120000000000002</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.9627</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1.4963</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1.1739999999999999</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0.75190000000000001</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0.66469999999999996</v>
+      </c>
+      <c r="H18" s="7">
+        <v>1.2858000000000001</v>
+      </c>
+      <c r="I18" s="7">
+        <v>1.5793999999999999</v>
+      </c>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="7">
+        <v>1.6943999999999999</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.60429999999999995</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1.0079</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.84589999999999999</v>
+      </c>
+      <c r="F19" s="7">
+        <v>2.3043</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1.4738</v>
+      </c>
+      <c r="H19" s="7">
+        <v>1.2156</v>
+      </c>
+      <c r="I19" s="7">
+        <v>0.67520000000000002</v>
+      </c>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" s="7">
+        <v>0.96930000000000005</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.83209999999999995</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1.8501000000000001</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.93489999999999995</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1.1086</v>
+      </c>
+      <c r="H20" s="7">
+        <v>1.3362000000000001</v>
+      </c>
+      <c r="I20" s="7">
+        <v>1.1647000000000001</v>
+      </c>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" s="7">
+        <v>2.3016999999999999</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1.2674000000000001</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.6966</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1.2364999999999999</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.77669999999999995</v>
+      </c>
+      <c r="G21" s="7">
+        <v>1.2339</v>
+      </c>
+      <c r="H21" s="7">
+        <v>2.5449999999999999</v>
+      </c>
+      <c r="I21" s="7">
+        <v>1.335</v>
+      </c>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" s="7">
+        <v>1.5911</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1.1839999999999999</v>
+      </c>
+      <c r="D22" s="7">
+        <v>2.9990999999999999</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1.4118999999999999</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0.84909999999999997</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1.3825000000000001</v>
+      </c>
+      <c r="H22" s="7">
+        <v>2.3018999999999998</v>
+      </c>
+      <c r="I22" s="7">
+        <v>1.1417999999999999</v>
+      </c>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" s="7">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.69189999999999996</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2.4199000000000002</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1.3884000000000001</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0.18410000000000001</v>
+      </c>
+      <c r="G23" s="7">
+        <v>0.99029999999999996</v>
+      </c>
+      <c r="H23" s="7">
+        <v>1.8383</v>
+      </c>
+      <c r="I23" s="7">
+        <v>1.71</v>
+      </c>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" s="7">
+        <v>1.6475</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.49180000000000001</v>
+      </c>
+      <c r="D24" s="7">
+        <v>1.7309000000000001</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.73570000000000002</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0.64419999999999999</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0.97689999999999999</v>
+      </c>
+      <c r="H24" s="7">
+        <v>1.1094999999999999</v>
+      </c>
+      <c r="I24" s="7">
+        <v>2.0451999999999999</v>
+      </c>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" s="7">
+        <v>1.3322000000000001</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.75229999999999997</v>
+      </c>
+      <c r="D25" s="7">
+        <v>3.0945999999999998</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1.5637000000000001</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0.94359999999999999</v>
+      </c>
+      <c r="G25" s="7">
+        <v>1.1459999999999999</v>
+      </c>
+      <c r="H25" s="7">
+        <v>1.3008</v>
+      </c>
+      <c r="I25" s="7">
+        <v>1.4435</v>
+      </c>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" s="7">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0.74380000000000002</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1.4345000000000001</v>
+      </c>
+      <c r="E26" s="7">
+        <v>1.5147999999999999</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0.73429999999999995</v>
+      </c>
+      <c r="G26" s="7">
+        <v>1.7514000000000001</v>
+      </c>
+      <c r="H26" s="7">
+        <v>1.4323999999999999</v>
+      </c>
+      <c r="I26" s="7">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" s="7">
+        <v>1.3515999999999999</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0.70409999999999995</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1.5135000000000001</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.46529999999999999</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0.53849999999999998</v>
+      </c>
+      <c r="H27" s="7">
+        <v>0.70289999999999997</v>
+      </c>
+      <c r="I27" s="7">
+        <v>0.78610000000000002</v>
+      </c>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" s="7">
+        <v>0.60450000000000004</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0.83560000000000001</v>
+      </c>
+      <c r="D28" s="7">
+        <v>2.3984000000000001</v>
+      </c>
+      <c r="E28" s="7">
+        <v>1.2193000000000001</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0.71060000000000001</v>
+      </c>
+      <c r="G28" s="7">
+        <v>1.7908999999999999</v>
+      </c>
+      <c r="H28" s="7">
+        <v>1.4623999999999999</v>
+      </c>
+      <c r="I28" s="7">
+        <v>1.0894999999999999</v>
+      </c>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" s="7">
+        <v>1.0837000000000001</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0.9819</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1.7271000000000001</v>
+      </c>
+      <c r="E29" s="7">
+        <v>1.0606</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0.68459999999999999</v>
+      </c>
+      <c r="G29" s="7">
+        <v>1.206</v>
+      </c>
+      <c r="H29" s="7">
+        <v>2.1909999999999998</v>
+      </c>
+      <c r="I29" s="7">
+        <v>1.3903000000000001</v>
+      </c>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" s="7">
+        <v>1.5241</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0.79920000000000002</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0.95520000000000005</v>
+      </c>
+      <c r="E30" s="7">
+        <v>1.4751000000000001</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0.81389999999999996</v>
+      </c>
+      <c r="G30" s="7">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="H30" s="7">
+        <v>2.0947</v>
+      </c>
+      <c r="I30" s="7">
+        <v>0.80969999999999998</v>
+      </c>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7">
+        <v>2.0112999999999999</v>
+      </c>
+      <c r="C31" s="7">
+        <v>0.59819999999999995</v>
+      </c>
+      <c r="D31" s="7">
+        <v>0.66820000000000002</v>
+      </c>
+      <c r="E31" s="7">
+        <v>1.2083999999999999</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0.51229999999999998</v>
+      </c>
+      <c r="G31" s="7">
+        <v>0.98089999999999999</v>
+      </c>
+      <c r="H31" s="7">
+        <v>1.2010000000000001</v>
+      </c>
+      <c r="I31" s="7">
+        <v>1.0525</v>
+      </c>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B32" s="7">
+        <v>1.1760999999999999</v>
+      </c>
+      <c r="C32" s="7">
+        <v>1.0798000000000001</v>
+      </c>
+      <c r="D32" s="7">
+        <v>2.0634000000000001</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0.97770000000000001</v>
+      </c>
+      <c r="F32" s="7">
+        <v>2.3016000000000001</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1.4907999999999999</v>
+      </c>
+      <c r="H32" s="7">
+        <v>1.7910999999999999</v>
+      </c>
+      <c r="I32" s="7">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H33" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B33" s="7">
+        <v>0.3231</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="D33" s="7">
+        <v>3.4841000000000002</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0.97770000000000001</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="G33" s="7">
+        <v>0.77659999999999996</v>
+      </c>
+      <c r="H33" s="7">
+        <v>0.82830000000000004</v>
+      </c>
+      <c r="I33" s="7">
+        <v>1.6311</v>
+      </c>
+      <c r="J33" s="7"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" t="s">
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
-        <v>1</v>
-      </c>
-      <c r="H34" t="s">
-        <v>1</v>
-      </c>
-      <c r="I34" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="7">
+        <v>0.22850000000000001</v>
+      </c>
+      <c r="C34" s="7">
+        <v>0.52890000000000004</v>
+      </c>
+      <c r="D34" s="7">
+        <v>2.6497000000000002</v>
+      </c>
+      <c r="E34" s="7">
+        <v>1.2354000000000001</v>
+      </c>
+      <c r="F34" s="7">
+        <v>1.3621000000000001</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1.0245</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0.44059999999999999</v>
+      </c>
+      <c r="I34" s="7">
+        <v>1.0436000000000001</v>
+      </c>
+      <c r="J34" s="7"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="7">
+        <v>0.27979999999999999</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.3735</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0.43319999999999997</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0.93210000000000004</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0.74560000000000004</v>
+      </c>
+      <c r="G35" s="7">
+        <v>0.85260000000000002</v>
+      </c>
+      <c r="H35" s="7">
+        <v>1.7758</v>
+      </c>
+      <c r="I35" s="7">
+        <v>1.0143</v>
+      </c>
+      <c r="J35" s="7"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B36" s="7">
+        <v>2.0047999999999999</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0.81410000000000005</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1.7271000000000001</v>
+      </c>
+      <c r="E36" s="7">
+        <v>1.2733000000000001</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0.88780000000000003</v>
+      </c>
+      <c r="G36" s="7">
+        <v>0.81369999999999998</v>
+      </c>
+      <c r="H36" s="7">
+        <v>1.4023000000000001</v>
+      </c>
+      <c r="I36" s="7">
+        <v>1.0143</v>
+      </c>
+      <c r="J36" s="7"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="7">
+        <v>0.22850000000000001</v>
+      </c>
+      <c r="C37" s="7">
+        <v>1.1303000000000001</v>
+      </c>
+      <c r="D37" s="7">
+        <v>1.7605</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0.45669999999999999</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0.59219999999999995</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1.1880999999999999</v>
+      </c>
+      <c r="H37" s="7">
+        <v>2.0310999999999999</v>
+      </c>
+      <c r="I37" s="7">
+        <v>0.59830000000000005</v>
+      </c>
+      <c r="J37" s="7"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="7">
+        <v>1.7844</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0.67279999999999995</v>
+      </c>
+      <c r="D38" s="7">
+        <v>1.3886000000000001</v>
+      </c>
+      <c r="E38" s="7">
+        <v>1.3586</v>
+      </c>
+      <c r="F38" s="7">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="G38" s="7">
+        <v>0.94320000000000004</v>
+      </c>
+      <c r="H38" s="7">
+        <v>1.6758999999999999</v>
+      </c>
+      <c r="I38" s="7">
+        <v>1.5444</v>
+      </c>
+      <c r="J38" s="7"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B39" s="7">
+        <v>1.0837000000000001</v>
+      </c>
+      <c r="C39" s="7">
+        <v>1.3398000000000001</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0.53959999999999997</v>
+      </c>
+      <c r="E39" s="7">
+        <v>1.4007000000000001</v>
+      </c>
+      <c r="F39" s="7">
+        <v>0.3483</v>
+      </c>
+      <c r="G39" s="7">
+        <v>1.1538999999999999</v>
+      </c>
+      <c r="H39" s="7">
+        <v>1.3149999999999999</v>
+      </c>
+      <c r="I39" s="7">
+        <v>1.1234999999999999</v>
+      </c>
+      <c r="J39" s="7"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B40" s="7">
+        <v>0.68540000000000001</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0.97009999999999996</v>
+      </c>
+      <c r="D40" s="7">
+        <v>2.1615000000000002</v>
+      </c>
+      <c r="E40" s="7">
+        <v>1.1875</v>
+      </c>
+      <c r="F40" s="7">
+        <v>2.4152</v>
+      </c>
+      <c r="G40" s="7">
+        <v>1.1959</v>
+      </c>
+      <c r="H40" s="7">
+        <v>1.8502000000000001</v>
+      </c>
+      <c r="I40" s="7">
+        <v>1.2369000000000001</v>
+      </c>
+      <c r="J40" s="7"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B41" s="7">
+        <v>1.454</v>
+      </c>
+      <c r="C41" s="7">
+        <v>1.3789</v>
+      </c>
+      <c r="D41" s="7">
+        <v>3.2025000000000001</v>
+      </c>
+      <c r="E41" s="7">
+        <v>1.3170999999999999</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0.89910000000000001</v>
+      </c>
+      <c r="G41" s="7">
+        <v>1.5111000000000001</v>
+      </c>
+      <c r="H41" s="7">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="I41" s="7">
+        <v>1.1302000000000001</v>
+      </c>
+      <c r="J41" s="7"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B42" s="7">
+        <v>1.3025</v>
+      </c>
+      <c r="C42" s="7">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0.98519999999999996</v>
+      </c>
+      <c r="E42" s="7">
+        <v>1.2061999999999999</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1.2501</v>
+      </c>
+      <c r="G42" s="7">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="H42" s="7">
+        <v>1.6567000000000001</v>
+      </c>
+      <c r="I42" s="7">
+        <v>1.1728000000000001</v>
+      </c>
+      <c r="J42" s="7"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B43" s="7">
+        <v>1.1760999999999999</v>
+      </c>
+      <c r="C43" s="7">
+        <v>1.1162000000000001</v>
+      </c>
+      <c r="D43" s="7">
+        <v>0.96860000000000002</v>
+      </c>
+      <c r="E43" s="7">
+        <v>1.1695</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0.77510000000000001</v>
+      </c>
+      <c r="G43" s="7">
+        <v>0.93110000000000004</v>
+      </c>
+      <c r="H43" s="7">
+        <v>2.1732</v>
+      </c>
+      <c r="I43" s="7">
+        <v>1.0894999999999999</v>
+      </c>
+      <c r="J43" s="7"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B44" s="7">
+        <v>1.1872</v>
+      </c>
+      <c r="C44" s="7">
+        <v>0.97570000000000001</v>
+      </c>
+      <c r="D44" s="7">
+        <v>1.7568999999999999</v>
+      </c>
+      <c r="E44" s="7">
+        <v>1.1729000000000001</v>
+      </c>
+      <c r="F44" s="7">
+        <v>0.67120000000000002</v>
+      </c>
+      <c r="G44" s="7">
+        <v>0.41120000000000001</v>
+      </c>
+      <c r="H44" s="7">
+        <v>1.5401</v>
+      </c>
+      <c r="I44" s="7">
+        <v>1.1385000000000001</v>
+      </c>
+      <c r="J44" s="7"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B45" s="7">
+        <v>1.3025</v>
+      </c>
+      <c r="C45" s="7">
+        <v>1.3418000000000001</v>
+      </c>
+      <c r="D45" s="7">
+        <v>1.9851000000000001</v>
+      </c>
+      <c r="E45" s="7">
+        <v>0.75170000000000003</v>
+      </c>
+      <c r="F45" s="7">
+        <v>1.3714999999999999</v>
+      </c>
+      <c r="G45" s="7">
+        <v>1.3958999999999999</v>
+      </c>
+      <c r="H45" s="7">
+        <v>0.99480000000000002</v>
+      </c>
+      <c r="I45" s="7">
+        <v>1.1218999999999999</v>
+      </c>
+      <c r="J45" s="7"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B46" s="7">
+        <v>0.74029999999999996</v>
+      </c>
+      <c r="C46" s="7">
+        <v>0.48349999999999999</v>
+      </c>
+      <c r="D46" s="7">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="E46" s="7">
+        <v>1.0803</v>
+      </c>
+      <c r="F46" s="7">
+        <v>0.77680000000000005</v>
+      </c>
+      <c r="G46" s="7">
+        <v>0.77459999999999996</v>
+      </c>
+      <c r="H46" s="7">
+        <v>1.0961000000000001</v>
+      </c>
+      <c r="I46" s="7">
+        <v>0.61080000000000001</v>
+      </c>
+      <c r="J46" s="7"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B47" s="7">
+        <v>0.48470000000000002</v>
+      </c>
+      <c r="C47" s="7">
+        <v>0.95960000000000001</v>
+      </c>
+      <c r="D47" s="7">
+        <v>1.3120000000000001</v>
+      </c>
+      <c r="E47" s="7">
+        <v>1.0147999999999999</v>
+      </c>
+      <c r="F47" s="7">
+        <v>0.66059999999999997</v>
+      </c>
+      <c r="G47" s="7">
+        <v>0.49030000000000001</v>
+      </c>
+      <c r="H47" s="7">
+        <v>2.1993999999999998</v>
+      </c>
+      <c r="I47" s="7">
+        <v>1.4025000000000001</v>
+      </c>
+      <c r="J47" s="7"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" s="7">
+        <v>1.7474000000000001</v>
+      </c>
+      <c r="C48" s="7">
+        <v>1.3683000000000001</v>
+      </c>
+      <c r="D48" s="7">
+        <v>0.62309999999999999</v>
+      </c>
+      <c r="E48" s="7">
+        <v>0.89449999999999996</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0.59930000000000005</v>
+      </c>
+      <c r="G48" s="7">
+        <v>1.3001</v>
+      </c>
+      <c r="H48" s="7">
+        <v>1.4442999999999999</v>
+      </c>
+      <c r="I48" s="7">
+        <v>1.1451</v>
+      </c>
+      <c r="J48" s="7"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="C49" s="7">
+        <v>0.46650000000000003</v>
+      </c>
+      <c r="D49" s="7">
+        <v>0.7631</v>
+      </c>
+      <c r="E49" s="7">
+        <v>0.50609999999999999</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0.29289999999999999</v>
+      </c>
+      <c r="G49" s="7">
+        <v>0.76949999999999996</v>
+      </c>
+      <c r="H49" s="7">
+        <v>1.3154999999999999</v>
+      </c>
+      <c r="I49" s="7">
+        <v>1.1792</v>
+      </c>
+      <c r="J49" s="7"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" s="7">
+        <v>1.1872</v>
+      </c>
+      <c r="C50" s="7">
+        <v>1.1854</v>
+      </c>
+      <c r="D50" s="7">
+        <v>2.3342000000000001</v>
+      </c>
+      <c r="E50" s="7">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0.35320000000000001</v>
+      </c>
+      <c r="G50" s="7">
+        <v>0.89029999999999998</v>
+      </c>
+      <c r="H50" s="7">
+        <v>0.81540000000000001</v>
+      </c>
+      <c r="I50" s="7">
+        <v>0.78849999999999998</v>
+      </c>
+      <c r="J50" s="7"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" s="7">
+        <v>1.0217000000000001</v>
+      </c>
+      <c r="C51" s="7">
+        <v>0.59819999999999995</v>
+      </c>
+      <c r="D51" s="7">
+        <v>1.6367</v>
+      </c>
+      <c r="E51" s="7">
+        <v>1.0530999999999999</v>
+      </c>
+      <c r="F51" s="7">
+        <v>2.2877000000000001</v>
+      </c>
+      <c r="G51" s="7">
+        <v>0.75180000000000002</v>
+      </c>
+      <c r="H51" s="7">
+        <v>1.4784999999999999</v>
+      </c>
+      <c r="I51" s="7">
+        <v>2.0322</v>
+      </c>
+      <c r="J51" s="7"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" s="7">
+        <v>0.96930000000000005</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0.87660000000000005</v>
+      </c>
+      <c r="D52" s="7">
+        <v>0.93459999999999999</v>
+      </c>
+      <c r="E52" s="7">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="F52" s="7">
+        <v>0.19839999999999999</v>
+      </c>
+      <c r="G52" s="7">
+        <v>0.95630000000000004</v>
+      </c>
+      <c r="H52" s="7">
+        <v>0.27279999999999999</v>
+      </c>
+      <c r="I52" s="7">
+        <v>0.96079999999999999</v>
+      </c>
+      <c r="J52" s="7"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" s="7">
+        <v>2.0434999999999999</v>
+      </c>
+      <c r="C53" s="7">
+        <v>0.5131</v>
+      </c>
+      <c r="D53" s="7">
+        <v>0.75029999999999997</v>
+      </c>
+      <c r="E53" s="7">
+        <v>0.75349999999999995</v>
+      </c>
+      <c r="F53" s="7">
+        <v>0.75639999999999996</v>
+      </c>
+      <c r="G53" s="7">
+        <v>0.75119999999999998</v>
+      </c>
+      <c r="H53" s="7">
+        <v>1.2809999999999999</v>
+      </c>
+      <c r="I53" s="7">
+        <v>2.1131000000000002</v>
+      </c>
+      <c r="J53" s="7"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" s="7">
+        <v>1.2089000000000001</v>
+      </c>
+      <c r="C54" s="7">
+        <v>1.3787</v>
+      </c>
+      <c r="D54" s="7">
+        <v>0.5151</v>
+      </c>
+      <c r="E54" s="7">
+        <v>0.65610000000000002</v>
+      </c>
+      <c r="F54" s="7">
+        <v>0.3322</v>
+      </c>
+      <c r="G54" s="7">
+        <v>0.38719999999999999</v>
+      </c>
+      <c r="H54" s="7">
+        <v>2.2187000000000001</v>
+      </c>
+      <c r="I54" s="7">
+        <v>1.9314</v>
+      </c>
+      <c r="J54" s="7"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" s="7">
+        <v>0.48470000000000002</v>
+      </c>
+      <c r="C55" s="7">
+        <v>1.2163999999999999</v>
+      </c>
+      <c r="D55" s="7">
+        <v>1.0301</v>
+      </c>
+      <c r="E55" s="7">
+        <v>0.57909999999999995</v>
+      </c>
+      <c r="F55" s="7">
+        <v>0.36830000000000002</v>
+      </c>
+      <c r="G55" s="7">
+        <v>1.0335000000000001</v>
+      </c>
+      <c r="H55" s="7">
+        <v>1.5343</v>
+      </c>
+      <c r="I55" s="7">
+        <v>1.0738000000000001</v>
+      </c>
+      <c r="J55" s="7"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" s="7">
+        <v>1.5067999999999999</v>
+      </c>
+      <c r="C56" s="7">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="D56" s="7">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="E56" s="7">
+        <v>1.3351</v>
+      </c>
+      <c r="F56" s="7">
+        <v>1.4863</v>
+      </c>
+      <c r="G56" s="7">
+        <v>1.3929</v>
+      </c>
+      <c r="H56" s="7">
+        <v>1.4136</v>
+      </c>
+      <c r="I56" s="7">
+        <v>1.8680000000000001</v>
+      </c>
+      <c r="J56" s="7"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" s="7">
+        <v>0.68540000000000001</v>
+      </c>
+      <c r="C57" s="7">
+        <v>0.95879999999999999</v>
+      </c>
+      <c r="D57" s="7">
+        <v>0.1799</v>
+      </c>
+      <c r="E57" s="7">
+        <v>1.3547</v>
+      </c>
+      <c r="F57" s="7">
+        <v>0.49349999999999999</v>
+      </c>
+      <c r="G57" s="7">
+        <v>0.7056</v>
+      </c>
+      <c r="H57" s="7">
+        <v>1.0879000000000001</v>
+      </c>
+      <c r="I57" s="7">
+        <v>1.1981999999999999</v>
+      </c>
+      <c r="J57" s="7"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" s="7">
+        <v>1.5067999999999999</v>
+      </c>
+      <c r="C58" s="7">
+        <v>0.65469999999999995</v>
+      </c>
+      <c r="D58" s="7">
+        <v>1.1958</v>
+      </c>
+      <c r="E58" s="7">
+        <v>0.62090000000000001</v>
+      </c>
+      <c r="F58" s="7">
+        <v>0.99629999999999996</v>
+      </c>
+      <c r="G58" s="7">
+        <v>1.7749999999999999</v>
+      </c>
+      <c r="H58" s="7">
+        <v>1.0137</v>
+      </c>
+      <c r="I58" s="7">
+        <v>1.2565</v>
+      </c>
+      <c r="J58" s="7"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" s="7">
+        <v>0.48470000000000002</v>
+      </c>
+      <c r="C59" s="7">
+        <v>1.2432000000000001</v>
+      </c>
+      <c r="D59" s="7">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="E59" s="7">
+        <v>1.6800999999999999</v>
+      </c>
+      <c r="F59" s="7">
+        <v>0.29320000000000002</v>
+      </c>
+      <c r="G59" s="7">
+        <v>1.3968</v>
+      </c>
+      <c r="H59" s="7">
+        <v>2.5350999999999999</v>
+      </c>
+      <c r="I59" s="7">
+        <v>1.5247999999999999</v>
+      </c>
+      <c r="J59" s="7"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" s="7">
+        <v>1.8771</v>
+      </c>
+      <c r="C60" s="7">
+        <v>0.43469999999999998</v>
+      </c>
+      <c r="D60" s="7">
+        <v>0.63849999999999996</v>
+      </c>
+      <c r="E60" s="7">
+        <v>1.3835999999999999</v>
+      </c>
+      <c r="F60" s="7">
+        <v>1.6789000000000001</v>
+      </c>
+      <c r="G60" s="7">
+        <v>1.5398000000000001</v>
+      </c>
+      <c r="H60" s="7">
+        <v>0.89739999999999998</v>
+      </c>
+      <c r="I60" s="7">
+        <v>1.1533</v>
+      </c>
+      <c r="J60" s="7"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" s="7">
+        <v>1.1423000000000001</v>
+      </c>
+      <c r="C61" s="7">
+        <v>0.38729999999999998</v>
+      </c>
+      <c r="D61" s="7">
+        <v>2.0508000000000002</v>
+      </c>
+      <c r="E61" s="7">
+        <v>1.7704</v>
+      </c>
+      <c r="F61" s="7">
+        <v>0.85980000000000001</v>
+      </c>
+      <c r="G61" s="7">
+        <v>1.8178000000000001</v>
+      </c>
+      <c r="H61" s="7">
+        <v>1.3823000000000001</v>
+      </c>
+      <c r="I61" s="7">
+        <v>0.77159999999999995</v>
+      </c>
+      <c r="J61" s="7"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" s="7">
+        <v>0.6462</v>
+      </c>
+      <c r="C62" s="7">
+        <v>0.97689999999999999</v>
+      </c>
+      <c r="D62" s="7">
+        <v>1.0549999999999999</v>
+      </c>
+      <c r="E62" s="7">
+        <v>0.77080000000000004</v>
+      </c>
+      <c r="F62" s="7">
+        <v>1.2524</v>
+      </c>
+      <c r="G62" s="7">
+        <v>0.64790000000000003</v>
+      </c>
+      <c r="H62" s="7">
+        <v>0.58789999999999998</v>
+      </c>
+      <c r="I62" s="7">
+        <v>0.88959999999999995</v>
+      </c>
+      <c r="J62" s="7"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" s="7">
+        <v>1.5992999999999999</v>
+      </c>
+      <c r="C63" s="7">
+        <v>0.4466</v>
+      </c>
+      <c r="D63" s="7">
+        <v>1.9539</v>
+      </c>
+      <c r="E63" s="7">
+        <v>0.8841</v>
+      </c>
+      <c r="F63" s="7">
+        <v>0.71309999999999996</v>
+      </c>
+      <c r="G63" s="7">
+        <v>1.0965</v>
+      </c>
+      <c r="H63" s="7">
+        <v>1.2988</v>
+      </c>
+      <c r="I63" s="7">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="J63" s="7"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" s="7">
+        <v>0.51090000000000002</v>
+      </c>
+      <c r="C64" s="7">
+        <v>1.9197</v>
+      </c>
+      <c r="D64" s="7">
+        <v>1.0971</v>
+      </c>
+      <c r="E64" s="7">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="F64" s="7">
+        <v>1.0511999999999999</v>
+      </c>
+      <c r="G64" s="7">
+        <v>0.98629999999999995</v>
+      </c>
+      <c r="H64" s="7">
+        <v>0.78269999999999995</v>
+      </c>
+      <c r="I64" s="7">
+        <v>0.88959999999999995</v>
+      </c>
+      <c r="J64" s="7"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" s="7">
+        <v>0.66610000000000003</v>
+      </c>
+      <c r="C65" s="7">
+        <v>1.1623000000000001</v>
+      </c>
+      <c r="D65" s="7">
+        <v>1.0882000000000001</v>
+      </c>
+      <c r="E65" s="7">
+        <v>1.4679</v>
+      </c>
+      <c r="F65" s="7">
+        <v>0.79090000000000005</v>
+      </c>
+      <c r="G65" s="7">
+        <v>1.1518999999999999</v>
+      </c>
+      <c r="H65" s="7">
+        <v>1.6857</v>
+      </c>
+      <c r="I65" s="7">
+        <v>1.7383999999999999</v>
+      </c>
+      <c r="J65" s="7"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" s="7">
+        <v>1.8839999999999999</v>
+      </c>
+      <c r="C66" s="7">
+        <v>0.59570000000000001</v>
+      </c>
+      <c r="D66" s="7">
+        <v>0.61260000000000003</v>
+      </c>
+      <c r="E66" s="7">
+        <v>1.1009</v>
+      </c>
+      <c r="F66" s="7">
+        <v>0.4133</v>
+      </c>
+      <c r="G66" s="7">
+        <v>2.4432999999999998</v>
+      </c>
+      <c r="H66" s="7">
+        <v>1.6588000000000001</v>
+      </c>
+      <c r="I66" s="7">
+        <v>1.571</v>
+      </c>
+      <c r="J66" s="7"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" s="7">
+        <v>1.0344</v>
+      </c>
+      <c r="C67" s="7">
+        <v>1.3252999999999999</v>
+      </c>
+      <c r="D67" s="7">
+        <v>0.62829999999999997</v>
+      </c>
+      <c r="E67" s="7">
+        <v>0.82540000000000002</v>
+      </c>
+      <c r="F67" s="7">
+        <v>0.82179999999999997</v>
+      </c>
+      <c r="G67" s="7">
+        <v>1.3066</v>
+      </c>
+      <c r="H67" s="7">
+        <v>1.5186999999999999</v>
+      </c>
+      <c r="I67" s="7">
+        <v>1.1597999999999999</v>
+      </c>
+      <c r="J67" s="7"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" s="7">
+        <v>0.62570000000000003</v>
+      </c>
+      <c r="C68" s="7">
+        <v>1.675</v>
+      </c>
+      <c r="D68" s="7">
+        <v>2.2608999999999999</v>
+      </c>
+      <c r="E68" s="7">
+        <v>0.52149999999999996</v>
+      </c>
+      <c r="F68" s="7">
+        <v>0.10929999999999999</v>
+      </c>
+      <c r="G68" s="7">
+        <v>0.60489999999999999</v>
+      </c>
+      <c r="H68" s="7">
+        <v>0.99539999999999995</v>
+      </c>
+      <c r="I68" s="7">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J68" s="7"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <f t="shared" ref="A69:A102" si="1">A68+1</f>
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" s="7">
+        <v>0</v>
+      </c>
+      <c r="C69" s="7">
+        <v>0.97729999999999995</v>
+      </c>
+      <c r="D69" s="7">
+        <v>1.6564000000000001</v>
+      </c>
+      <c r="E69" s="7">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="F69" s="7">
+        <v>0.88919999999999999</v>
+      </c>
+      <c r="G69" s="7">
+        <v>1.3127</v>
+      </c>
+      <c r="H69" s="7">
+        <v>1.8709</v>
+      </c>
+      <c r="I69" s="7">
+        <v>1.0105</v>
+      </c>
+      <c r="J69" s="7"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" s="7">
+        <v>1.952</v>
+      </c>
+      <c r="C70" s="7">
+        <v>1.4157999999999999</v>
+      </c>
+      <c r="D70" s="7">
+        <v>2.3216999999999999</v>
+      </c>
+      <c r="E70" s="7">
+        <v>0.77590000000000003</v>
+      </c>
+      <c r="F70" s="7">
+        <v>1.097</v>
+      </c>
+      <c r="G70" s="7">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="H70" s="7">
+        <v>1.6748000000000001</v>
+      </c>
+      <c r="I70" s="7">
+        <v>1.2655000000000001</v>
+      </c>
+      <c r="J70" s="7"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" s="7">
+        <v>1.6235999999999999</v>
+      </c>
+      <c r="C71" s="7">
+        <v>0.99919999999999998</v>
+      </c>
+      <c r="D71" s="7">
+        <v>1.7215</v>
+      </c>
+      <c r="E71" s="7">
+        <v>1.0004</v>
+      </c>
+      <c r="F71" s="7">
+        <v>0.9133</v>
+      </c>
+      <c r="G71" s="7">
+        <v>0.90139999999999998</v>
+      </c>
+      <c r="H71" s="7">
+        <v>1.7988</v>
+      </c>
+      <c r="I71" s="7">
+        <v>1.4225000000000001</v>
+      </c>
+      <c r="J71" s="7"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" s="7">
+        <v>1.1309</v>
+      </c>
+      <c r="C72" s="7">
+        <v>0.81240000000000001</v>
+      </c>
+      <c r="D72" s="7">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="E72" s="7">
+        <v>1.5746</v>
+      </c>
+      <c r="F72" s="7">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="G72" s="7">
+        <v>0.46</v>
+      </c>
+      <c r="H72" s="7">
+        <v>1.8635999999999999</v>
+      </c>
+      <c r="I72" s="7">
+        <v>1.0579000000000001</v>
+      </c>
+      <c r="J72" s="7"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" s="7">
+        <v>0.83940000000000003</v>
+      </c>
+      <c r="C73" s="7">
+        <v>0.78159999999999996</v>
+      </c>
+      <c r="D73" s="7">
+        <v>1.8466</v>
+      </c>
+      <c r="E73" s="7">
+        <v>0.34849999999999998</v>
+      </c>
+      <c r="F73" s="7">
+        <v>0.80859999999999999</v>
+      </c>
+      <c r="G73" s="7">
+        <v>0.59509999999999996</v>
+      </c>
+      <c r="H73" s="7">
+        <v>0.90590000000000004</v>
+      </c>
+      <c r="I73" s="7">
+        <v>1.6275999999999999</v>
+      </c>
+      <c r="J73" s="7"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" s="7">
+        <v>1.2721</v>
+      </c>
+      <c r="C74" s="7">
+        <v>1.234</v>
+      </c>
+      <c r="D74" s="7">
+        <v>1.492</v>
+      </c>
+      <c r="E74" s="7">
+        <v>0.83650000000000002</v>
+      </c>
+      <c r="F74" s="7">
+        <v>0.59960000000000002</v>
+      </c>
+      <c r="G74" s="7">
+        <v>0.5998</v>
+      </c>
+      <c r="H74" s="7">
+        <v>1.5782</v>
+      </c>
+      <c r="I74" s="7">
+        <v>1.6618999999999999</v>
+      </c>
+      <c r="J74" s="7"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" s="7">
+        <v>0.53580000000000005</v>
+      </c>
+      <c r="C75" s="7">
+        <v>0.49180000000000001</v>
+      </c>
+      <c r="D75" s="7">
+        <v>0.58560000000000001</v>
+      </c>
+      <c r="E75" s="7">
+        <v>1.3380000000000001</v>
+      </c>
+      <c r="F75" s="7">
+        <v>0.99319999999999997</v>
+      </c>
+      <c r="G75" s="7">
+        <v>0.6573</v>
+      </c>
+      <c r="H75" s="7">
+        <v>1.2551000000000001</v>
+      </c>
+      <c r="I75" s="7">
+        <v>0.81210000000000004</v>
+      </c>
+      <c r="J75" s="7"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" s="7">
+        <v>0.36120000000000002</v>
+      </c>
+      <c r="C76" s="7">
+        <v>1.5815999999999999</v>
+      </c>
+      <c r="D76" s="7">
+        <v>1.5804</v>
+      </c>
+      <c r="E76" s="7">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="F76" s="7">
+        <v>1.4721</v>
+      </c>
+      <c r="G76" s="7">
+        <v>1.5630999999999999</v>
+      </c>
+      <c r="H76" s="7">
+        <v>1.5337000000000001</v>
+      </c>
+      <c r="I76" s="7">
+        <v>0.96079999999999999</v>
+      </c>
+      <c r="J76" s="7"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" s="7">
+        <v>0.53580000000000005</v>
+      </c>
+      <c r="C77" s="7">
+        <v>1.5459000000000001</v>
+      </c>
+      <c r="D77" s="7">
+        <v>2.5169000000000001</v>
+      </c>
+      <c r="E77" s="7">
+        <v>1.0753999999999999</v>
+      </c>
+      <c r="F77" s="7">
+        <v>0.57620000000000005</v>
+      </c>
+      <c r="G77" s="7">
+        <v>1.7356</v>
+      </c>
+      <c r="H77" s="7">
+        <v>1.6141000000000001</v>
+      </c>
+      <c r="I77" s="7">
+        <v>1.6125</v>
+      </c>
+      <c r="J77" s="7"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" s="7">
+        <v>1.8062</v>
+      </c>
+      <c r="C78" s="7">
+        <v>1.0555000000000001</v>
+      </c>
+      <c r="D78" s="7">
+        <v>1.0851999999999999</v>
+      </c>
+      <c r="E78" s="7">
+        <v>1.0544</v>
+      </c>
+      <c r="F78" s="7">
+        <v>0.36630000000000001</v>
+      </c>
+      <c r="G78" s="7">
+        <v>0.99790000000000001</v>
+      </c>
+      <c r="H78" s="7">
+        <v>0.97060000000000002</v>
+      </c>
+      <c r="I78" s="7">
+        <v>0.78369999999999995</v>
+      </c>
+      <c r="J78" s="7"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" s="7">
+        <v>1.3322000000000001</v>
+      </c>
+      <c r="C79" s="7">
+        <v>0.71619999999999995</v>
+      </c>
+      <c r="D79" s="7">
+        <v>0.87749999999999995</v>
+      </c>
+      <c r="E79" s="7">
+        <v>1.3181</v>
+      </c>
+      <c r="F79" s="7">
+        <v>0.65849999999999997</v>
+      </c>
+      <c r="G79" s="7">
+        <v>0.84189999999999998</v>
+      </c>
+      <c r="H79" s="7">
+        <v>0.78029999999999999</v>
+      </c>
+      <c r="I79" s="7">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J79" s="7"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" s="7">
+        <v>2.1309999999999998</v>
+      </c>
+      <c r="C80" s="7">
+        <v>1.05</v>
+      </c>
+      <c r="D80" s="7">
+        <v>1.0851999999999999</v>
+      </c>
+      <c r="E80" s="7">
+        <v>0.82379999999999998</v>
+      </c>
+      <c r="F80" s="7">
+        <v>0.36570000000000003</v>
+      </c>
+      <c r="G80" s="7">
+        <v>1.2222999999999999</v>
+      </c>
+      <c r="H80" s="7">
+        <v>1.198</v>
+      </c>
+      <c r="I80" s="7">
+        <v>1.0843</v>
+      </c>
+      <c r="J80" s="7"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" s="7">
+        <v>1.0837000000000001</v>
+      </c>
+      <c r="C81" s="7">
+        <v>0.60140000000000005</v>
+      </c>
+      <c r="D81" s="7">
+        <v>0.8004</v>
+      </c>
+      <c r="E81" s="7">
+        <v>1.7181999999999999</v>
+      </c>
+      <c r="F81" s="7">
+        <v>0.56540000000000001</v>
+      </c>
+      <c r="G81" s="7">
+        <v>0.67849999999999999</v>
+      </c>
+      <c r="H81" s="7">
+        <v>2.5996000000000001</v>
+      </c>
+      <c r="I81" s="7">
+        <v>0.44269999999999998</v>
+      </c>
+      <c r="J81" s="7"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" s="7">
+        <v>1.7697000000000001</v>
+      </c>
+      <c r="C82" s="7">
+        <v>1.0246</v>
+      </c>
+      <c r="D82" s="7">
+        <v>0.75890000000000002</v>
+      </c>
+      <c r="E82" s="7">
+        <v>0.70079999999999998</v>
+      </c>
+      <c r="F82" s="7">
+        <v>0.4037</v>
+      </c>
+      <c r="G82" s="7">
+        <v>0.87039999999999995</v>
+      </c>
+      <c r="H82" s="7">
+        <v>1.5711999999999999</v>
+      </c>
+      <c r="I82" s="7">
+        <v>2.2804000000000002</v>
+      </c>
+      <c r="J82" s="7"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" s="7">
+        <v>1.4268000000000001</v>
+      </c>
+      <c r="C83" s="7">
+        <v>0.84179999999999999</v>
+      </c>
+      <c r="D83" s="7">
+        <v>2.0758999999999999</v>
+      </c>
+      <c r="E83" s="7">
+        <v>0.9627</v>
+      </c>
+      <c r="F83" s="7">
+        <v>0.73509999999999998</v>
+      </c>
+      <c r="G83" s="7">
+        <v>1.0610999999999999</v>
+      </c>
+      <c r="H83" s="7">
+        <v>1.9235</v>
+      </c>
+      <c r="I83" s="7">
+        <v>1.3250999999999999</v>
+      </c>
+      <c r="J83" s="7"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" s="7">
+        <v>1.6073999999999999</v>
+      </c>
+      <c r="C84" s="7">
+        <v>1.7476</v>
+      </c>
+      <c r="D84" s="7">
+        <v>2.1358999999999999</v>
+      </c>
+      <c r="E84" s="7">
+        <v>1.6045</v>
+      </c>
+      <c r="F84" s="7">
+        <v>0.52529999999999999</v>
+      </c>
+      <c r="G84" s="7">
+        <v>1.6760999999999999</v>
+      </c>
+      <c r="H84" s="7">
+        <v>0.97640000000000005</v>
+      </c>
+      <c r="I84" s="7">
+        <v>1.0105</v>
+      </c>
+      <c r="J84" s="7"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" s="7">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="C85" s="7">
+        <v>0.8538</v>
+      </c>
+      <c r="D85" s="7">
+        <v>1.1739999999999999</v>
+      </c>
+      <c r="E85" s="7">
+        <v>1.2948999999999999</v>
+      </c>
+      <c r="F85" s="7">
+        <v>0.50509999999999999</v>
+      </c>
+      <c r="G85" s="7">
+        <v>1.4686999999999999</v>
+      </c>
+      <c r="H85" s="7">
+        <v>1.7514000000000001</v>
+      </c>
+      <c r="I85" s="7">
+        <v>0.49869999999999998</v>
+      </c>
+      <c r="J85" s="7"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" s="7">
+        <v>1.7548999999999999</v>
+      </c>
+      <c r="C86" s="7">
+        <v>0.45650000000000002</v>
+      </c>
+      <c r="D86" s="7">
+        <v>1.5639000000000001</v>
+      </c>
+      <c r="E86" s="7">
+        <v>1.6403000000000001</v>
+      </c>
+      <c r="F86" s="7">
+        <v>1.1457999999999999</v>
+      </c>
+      <c r="G86" s="7">
+        <v>0.63549999999999995</v>
+      </c>
+      <c r="H86" s="7">
+        <v>1.0745</v>
+      </c>
+      <c r="I86" s="7">
+        <v>1.4025000000000001</v>
+      </c>
+      <c r="J86" s="7"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" s="7">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="C87" s="7">
+        <v>1.4093</v>
+      </c>
+      <c r="D87" s="7">
+        <v>1.7697000000000001</v>
+      </c>
+      <c r="E87" s="7">
+        <v>1.1081000000000001</v>
+      </c>
+      <c r="F87" s="7">
+        <v>1.5328999999999999</v>
+      </c>
+      <c r="G87" s="7">
+        <v>1.3569</v>
+      </c>
+      <c r="H87" s="7">
+        <v>0.62450000000000006</v>
+      </c>
+      <c r="I87" s="7">
+        <v>1.0143</v>
+      </c>
+      <c r="J87" s="7"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88" s="7">
+        <v>2.1554000000000002</v>
+      </c>
+      <c r="C88" s="7">
+        <v>0.7198</v>
+      </c>
+      <c r="D88" s="7">
+        <v>0.36859999999999998</v>
+      </c>
+      <c r="E88" s="7">
+        <v>1.0264</v>
+      </c>
+      <c r="F88" s="7">
+        <v>0.50680000000000003</v>
+      </c>
+      <c r="G88" s="7">
+        <v>1.2323999999999999</v>
+      </c>
+      <c r="H88" s="7">
+        <v>1.5717000000000001</v>
+      </c>
+      <c r="I88" s="7">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="J88" s="7"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" s="7">
+        <v>1.4450000000000001</v>
+      </c>
+      <c r="C89" s="7">
+        <v>1.1744000000000001</v>
+      </c>
+      <c r="D89" s="7">
+        <v>1.7063999999999999</v>
+      </c>
+      <c r="E89" s="7">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="F89" s="7">
+        <v>0.25940000000000002</v>
+      </c>
+      <c r="G89" s="7">
+        <v>0.95089999999999997</v>
+      </c>
+      <c r="H89" s="7">
+        <v>1.7016</v>
+      </c>
+      <c r="I89" s="7">
+        <v>1.3193999999999999</v>
+      </c>
+      <c r="J89" s="7"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" s="7">
+        <v>1.2197</v>
+      </c>
+      <c r="C90" s="7">
+        <v>0.75539999999999996</v>
+      </c>
+      <c r="D90" s="7">
+        <v>0.87749999999999995</v>
+      </c>
+      <c r="E90" s="7">
+        <v>1.448</v>
+      </c>
+      <c r="F90" s="7">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="G90" s="7">
+        <v>1.6386000000000001</v>
+      </c>
+      <c r="H90" s="7">
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="I90" s="7">
+        <v>1.1468</v>
+      </c>
+      <c r="J90" s="7"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" s="7">
+        <v>0.74029999999999996</v>
+      </c>
+      <c r="C91" s="7">
+        <v>1.5159</v>
+      </c>
+      <c r="D91" s="7">
+        <v>1.4963</v>
+      </c>
+      <c r="E91" s="7">
+        <v>1.3614999999999999</v>
+      </c>
+      <c r="F91" s="7">
+        <v>0.83340000000000003</v>
+      </c>
+      <c r="G91" s="7">
+        <v>1.3918999999999999</v>
+      </c>
+      <c r="H91" s="7">
+        <v>1.6189</v>
+      </c>
+      <c r="I91" s="7">
+        <v>0.626</v>
+      </c>
+      <c r="J91" s="7"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" s="7">
+        <v>1.1872</v>
+      </c>
+      <c r="C92" s="7">
+        <v>0.81789999999999996</v>
+      </c>
+      <c r="D92" s="7">
+        <v>1.9932000000000001</v>
+      </c>
+      <c r="E92" s="7">
+        <v>1.4258999999999999</v>
+      </c>
+      <c r="F92" s="7">
+        <v>1.0145</v>
+      </c>
+      <c r="G92" s="7">
+        <v>1.2785</v>
+      </c>
+      <c r="H92" s="7">
+        <v>0.47360000000000002</v>
+      </c>
+      <c r="I92" s="7">
+        <v>1.4947999999999999</v>
+      </c>
+      <c r="J92" s="7"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" s="7">
+        <v>1.4894000000000001</v>
+      </c>
+      <c r="C93" s="7">
+        <v>1.7008000000000001</v>
+      </c>
+      <c r="D93" s="7">
+        <v>2.4662999999999999</v>
+      </c>
+      <c r="E93" s="7">
+        <v>1.0936999999999999</v>
+      </c>
+      <c r="F93" s="7">
+        <v>1.6708000000000001</v>
+      </c>
+      <c r="G93" s="7">
+        <v>1.3609</v>
+      </c>
+      <c r="H93" s="7">
+        <v>1.0379</v>
+      </c>
+      <c r="I93" s="7">
+        <v>1.9305000000000001</v>
+      </c>
+      <c r="J93" s="7"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" s="7">
+        <v>0.45689999999999997</v>
+      </c>
+      <c r="C94" s="7">
+        <v>0.9819</v>
+      </c>
+      <c r="D94" s="7">
+        <v>1.9137</v>
+      </c>
+      <c r="E94" s="7">
+        <v>0.433</v>
+      </c>
+      <c r="F94" s="7">
+        <v>0.94130000000000003</v>
+      </c>
+      <c r="G94" s="7">
+        <v>1.3668</v>
+      </c>
+      <c r="H94" s="7">
+        <v>1.6065</v>
+      </c>
+      <c r="I94" s="7">
+        <v>0.72889999999999999</v>
+      </c>
+      <c r="J94" s="7"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" s="7">
+        <v>1.4450000000000001</v>
+      </c>
+      <c r="C95" s="7">
+        <v>0.62539999999999996</v>
+      </c>
+      <c r="D95" s="7">
+        <v>1.2304999999999999</v>
+      </c>
+      <c r="E95" s="7">
+        <v>1.6887000000000001</v>
+      </c>
+      <c r="F95" s="7">
+        <v>0.33429999999999999</v>
+      </c>
+      <c r="G95" s="7">
+        <v>1.7916000000000001</v>
+      </c>
+      <c r="H95" s="7">
+        <v>1.2362</v>
+      </c>
+      <c r="I95" s="7">
+        <v>0.66110000000000002</v>
+      </c>
+      <c r="J95" s="7"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B96" s="7">
+        <v>1.0716000000000001</v>
+      </c>
+      <c r="C96" s="7">
+        <v>1.6213</v>
+      </c>
+      <c r="D96" s="7">
+        <v>1.9120999999999999</v>
+      </c>
+      <c r="E96" s="7">
+        <v>0.89739999999999998</v>
+      </c>
+      <c r="F96" s="7">
+        <v>1.5226999999999999</v>
+      </c>
+      <c r="G96" s="7">
+        <v>1.1075999999999999</v>
+      </c>
+      <c r="H96" s="7">
+        <v>1.3801000000000001</v>
+      </c>
+      <c r="I96" s="7">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="J96" s="7"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B97" s="7">
+        <v>0.51090000000000002</v>
+      </c>
+      <c r="C97" s="7">
+        <v>0.84650000000000003</v>
+      </c>
+      <c r="D97" s="7">
+        <v>0.56879999999999997</v>
+      </c>
+      <c r="E97" s="7">
+        <v>1.1420999999999999</v>
+      </c>
+      <c r="F97" s="7">
+        <v>0.52929999999999999</v>
+      </c>
+      <c r="G97" s="7">
+        <v>0.91190000000000004</v>
+      </c>
+      <c r="H97" s="7">
+        <v>0.377</v>
+      </c>
+      <c r="I97" s="7">
+        <v>1.6676</v>
+      </c>
+      <c r="J97" s="7"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B98" s="7">
+        <v>0.82379999999999998</v>
+      </c>
+      <c r="C98" s="7">
+        <v>1.3874</v>
+      </c>
+      <c r="D98" s="7">
+        <v>2.5565000000000002</v>
+      </c>
+      <c r="E98" s="7">
+        <v>1.0901000000000001</v>
+      </c>
+      <c r="F98" s="7">
+        <v>0.64080000000000004</v>
+      </c>
+      <c r="G98" s="7">
+        <v>0.55420000000000003</v>
+      </c>
+      <c r="H98" s="7">
+        <v>2.4081999999999999</v>
+      </c>
+      <c r="I98" s="7">
+        <v>1.0086999999999999</v>
+      </c>
+      <c r="J98" s="7"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B99" s="7">
+        <v>0.82379999999999998</v>
+      </c>
+      <c r="C99" s="7">
+        <v>0.85809999999999997</v>
+      </c>
+      <c r="D99" s="7">
+        <v>0.91720000000000002</v>
+      </c>
+      <c r="E99" s="7">
+        <v>0.83020000000000005</v>
+      </c>
+      <c r="F99" s="7">
+        <v>1.0446</v>
+      </c>
+      <c r="G99" s="7">
+        <v>0.81989999999999996</v>
+      </c>
+      <c r="H99" s="7">
+        <v>2.7557999999999998</v>
+      </c>
+      <c r="I99" s="7">
+        <v>0.48330000000000001</v>
+      </c>
+      <c r="J99" s="7"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B100" s="7">
+        <v>1.3124</v>
+      </c>
+      <c r="C100" s="7">
+        <v>1.1315</v>
+      </c>
+      <c r="D100" s="7">
+        <v>1.714</v>
+      </c>
+      <c r="E100" s="7">
+        <v>1.1616</v>
+      </c>
+      <c r="F100" s="7">
+        <v>1.1640999999999999</v>
+      </c>
+      <c r="G100" s="7">
+        <v>1.0052000000000001</v>
+      </c>
+      <c r="H100" s="7">
+        <v>2.5169999999999999</v>
+      </c>
+      <c r="I100" s="7">
+        <v>1.1792</v>
+      </c>
+      <c r="J100" s="7"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B101" s="7">
+        <v>2.0497999999999998</v>
+      </c>
+      <c r="C101" s="7">
+        <v>0.48180000000000001</v>
+      </c>
+      <c r="D101" s="7">
+        <v>1.2358</v>
+      </c>
+      <c r="E101" s="7">
+        <v>0.80430000000000001</v>
+      </c>
+      <c r="F101" s="7">
+        <v>0.5988</v>
+      </c>
+      <c r="G101" s="7">
+        <v>1.0253000000000001</v>
+      </c>
+      <c r="H101" s="7">
+        <v>1.6856</v>
+      </c>
+      <c r="I101" s="7">
+        <v>0.72109999999999996</v>
+      </c>
+      <c r="J101" s="7"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B102" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="C102" s="7">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="D102" s="7">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="E102" s="7">
+        <v>1.0949</v>
+      </c>
+      <c r="F102" s="7">
+        <v>0.53169999999999995</v>
+      </c>
+      <c r="G102" s="7">
+        <v>1.3429</v>
+      </c>
+      <c r="H102" s="7">
+        <v>1.6507000000000001</v>
+      </c>
+      <c r="I102" s="7">
+        <v>1.0345</v>
+      </c>
+      <c r="J102" s="7"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B103" s="7"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="7"/>
+      <c r="I103" s="7"/>
+      <c r="J103" s="7"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B104" s="6">
         <f>SUM(B3:B102)/100</f>
-        <v>0</v>
+        <v>1.1278949999999999</v>
       </c>
       <c r="C104" s="6">
         <f t="shared" ref="C104:I104" si="2">SUM(C3:C102)/100</f>
-        <v>0</v>
+        <v>0.95918500000000018</v>
       </c>
       <c r="D104" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5104270000000002</v>
       </c>
       <c r="E104" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.0869840000000002</v>
       </c>
       <c r="F104" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.87630200000000003</v>
       </c>
       <c r="G104" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.1266000000000005</v>
       </c>
       <c r="H104" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.4430800000000001</v>
       </c>
       <c r="I104" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.1546240000000005</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
M=5 results and logs
</commit_message>
<xml_diff>
--- a/sessions/Mutiple Session Results - 29032022/Session Results (29th March 2022).xlsx
+++ b/sessions/Mutiple Session Results - 29032022/Session Results (29th March 2022).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\sessions\Mutiple Session Results - 29032022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D8BCF5-F820-45B2-ADD0-D93D2CEF4E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF269EED-A3BB-4069-956B-C82C16BB1431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M=1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="11">
   <si>
     <t>Number Of Times Pregnant</t>
   </si>
@@ -144,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -165,6 +165,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -449,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R104"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="H108" sqref="H108"/>
     </sheetView>
   </sheetViews>
@@ -9995,7 +9998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E31B93-D821-4DD2-B907-DCA43FD0730B}">
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
@@ -13201,10 +13204,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E593DE3-4F0A-4F22-98BD-01BD8440CE88}">
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13212,7 +13215,7 @@
     <col min="1" max="9" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -13241,7 +13244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -13254,670 +13257,3151 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="8">
+        <v>1.4805999999999999</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.62580000000000002</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.98909999999999998</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1.1498999999999999</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.8841</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.54569999999999996</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1.6707000000000001</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1.9985999999999999</v>
+      </c>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f>A3+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="8">
+        <v>1.7579</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.48609999999999998</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1.7958000000000001</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1.1444000000000001</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.66910000000000003</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1.1203000000000001</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1.4227000000000001</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.81989999999999996</v>
+      </c>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" ref="A5:A70" si="0">A4+1</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="8">
+        <v>1.6789000000000001</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.9852000000000001</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2.5811000000000002</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.39269999999999999</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.65869999999999995</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1.2271000000000001</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1.5931999999999999</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1.5712999999999999</v>
+      </c>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="8">
+        <v>1.1738999999999999</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1.2253000000000001</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1.0021</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.8841</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.87919999999999998</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1.3423</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1.7958000000000001</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1.0518000000000001</v>
+      </c>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="8">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1.3882000000000001</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.92979999999999996</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1.0670999999999999</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.78</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1.0825</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="I7" s="8">
+        <v>1.0019</v>
+      </c>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="8">
+        <v>1.2002999999999999</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.81240000000000001</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.92979999999999996</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1.2468999999999999</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1.1676</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1.0235000000000001</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1.5227999999999999</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1.4105000000000001</v>
+      </c>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="8">
+        <v>0.75080000000000002</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1.4965999999999999</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.73370000000000002</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1.282</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1.6533</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0.81989999999999996</v>
+      </c>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="8">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1.2354000000000001</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1.9769000000000001</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.69089999999999996</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.8931</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1.0008999999999999</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1.7746</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1.2746999999999999</v>
+      </c>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="8">
+        <v>1.2430000000000001</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.76959999999999995</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1.1420999999999999</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.73819999999999997</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.74670000000000003</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1.3364</v>
+      </c>
+      <c r="H11" s="8">
+        <v>2.0728</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1.2351000000000001</v>
+      </c>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="8">
+        <v>0.5958</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1.1495</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1.5861000000000001</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1.1472</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.43209999999999998</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1.6388</v>
+      </c>
+      <c r="H12" s="8">
+        <v>2.0867</v>
+      </c>
+      <c r="I12" s="8">
+        <v>2.5434999999999999</v>
+      </c>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="8">
+        <v>0.77810000000000001</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.65549999999999997</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.54790000000000005</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.93969999999999998</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1.3635999999999999</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.94169999999999998</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1.6257999999999999</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.83630000000000004</v>
+      </c>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="8">
+        <v>1.165</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1.0435000000000001</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1.8995</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.98360000000000003</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1.3698999999999999</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0.69020000000000004</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1.5359</v>
+      </c>
+      <c r="I14" s="8">
+        <v>1.224</v>
+      </c>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="8">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.51680000000000004</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2.1463999999999999</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.79469999999999996</v>
+      </c>
+      <c r="F15" s="8">
+        <v>2.2256999999999998</v>
+      </c>
+      <c r="G15" s="8">
+        <v>1.2768999999999999</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1.6155999999999999</v>
+      </c>
+      <c r="I15" s="8">
+        <v>1.2556</v>
+      </c>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" s="8">
+        <v>1.1738999999999999</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.60750000000000004</v>
+      </c>
+      <c r="D16" s="8">
+        <v>3.3485</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1.3963000000000001</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.57210000000000005</v>
+      </c>
+      <c r="G16" s="8">
+        <v>2.0211999999999999</v>
+      </c>
+      <c r="H16" s="8">
+        <v>1.5678000000000001</v>
+      </c>
+      <c r="I16" s="8">
+        <v>1.2544</v>
+      </c>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="8">
+        <v>0.5958</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.61529999999999996</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1.6500999999999999</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1.0818000000000001</v>
+      </c>
+      <c r="F17" s="8">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="G17" s="8">
+        <v>1.1465000000000001</v>
+      </c>
+      <c r="H17" s="8">
+        <v>1.7013</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0.9667</v>
+      </c>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" s="8">
+        <v>2.0537000000000001</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1.6607000000000001</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1.6072</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1.1012</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.67849999999999999</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1.5488999999999999</v>
+      </c>
+      <c r="H18" s="8">
+        <v>2.0880000000000001</v>
+      </c>
+      <c r="I18" s="8">
+        <v>1.6444000000000001</v>
+      </c>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="8">
+        <v>1.4805999999999999</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1.2630999999999999</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1.6641999999999999</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1.3209</v>
+      </c>
+      <c r="F19" s="8">
+        <v>2.1421000000000001</v>
+      </c>
+      <c r="G19" s="8">
+        <v>1.0026999999999999</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1.7345999999999999</v>
+      </c>
+      <c r="I19" s="8">
+        <v>1.0518000000000001</v>
+      </c>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" s="8">
+        <v>1.9278</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1.1746000000000001</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1.7476</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1.6987000000000001</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="G20" s="8">
+        <v>1.6498999999999999</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0.76439999999999997</v>
+      </c>
+      <c r="I20" s="8">
+        <v>1.1464000000000001</v>
+      </c>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" s="8">
+        <v>0.62980000000000003</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1.0284</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1.8980999999999999</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0.67549999999999999</v>
+      </c>
+      <c r="F21" s="8">
+        <v>2.0756999999999999</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.92459999999999998</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="I21" s="8">
+        <v>1.724</v>
+      </c>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" s="8">
+        <v>0.70789999999999997</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1.2455000000000001</v>
+      </c>
+      <c r="D22" s="8">
+        <v>2.8706999999999998</v>
+      </c>
+      <c r="E22" s="8">
+        <v>1.0174000000000001</v>
+      </c>
+      <c r="F22" s="8">
+        <v>1.9576</v>
+      </c>
+      <c r="G22" s="8">
+        <v>1.2983</v>
+      </c>
+      <c r="H22" s="8">
+        <v>1.6579999999999999</v>
+      </c>
+      <c r="I22" s="8">
+        <v>1.0730999999999999</v>
+      </c>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" s="8">
+        <v>2.0689000000000002</v>
+      </c>
+      <c r="C23" s="8">
+        <v>1.4014</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.84209999999999996</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0.7339</v>
+      </c>
+      <c r="F23" s="8">
+        <v>1.3099000000000001</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.90310000000000001</v>
+      </c>
+      <c r="H23" s="8">
+        <v>1.9843</v>
+      </c>
+      <c r="I23" s="8">
+        <v>1.1212</v>
+      </c>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" s="8">
+        <v>0.73680000000000001</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0.60470000000000002</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0.90439999999999998</v>
+      </c>
+      <c r="E24" s="8">
+        <v>1.07</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="G24" s="8">
+        <v>1.1809000000000001</v>
+      </c>
+      <c r="H24" s="8">
+        <v>2.4994999999999998</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0.9698</v>
+      </c>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" s="8">
+        <v>1.9547000000000001</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1.5581</v>
+      </c>
+      <c r="E25" s="8">
+        <v>1.4424999999999999</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.73780000000000001</v>
+      </c>
+      <c r="G25" s="8">
+        <v>1.1383000000000001</v>
+      </c>
+      <c r="H25" s="8">
+        <v>2.2387999999999999</v>
+      </c>
+      <c r="I25" s="8">
+        <v>1.6306</v>
+      </c>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" s="8">
+        <v>1.74</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.96819999999999995</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0.77159999999999995</v>
+      </c>
+      <c r="E26" s="8">
+        <v>1.2527999999999999</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0.69040000000000001</v>
+      </c>
+      <c r="G26" s="8">
+        <v>0.90359999999999996</v>
+      </c>
+      <c r="H26" s="8">
+        <v>1.4414</v>
+      </c>
+      <c r="I26" s="8">
+        <v>2.5594000000000001</v>
+      </c>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" s="8">
+        <v>0.4335</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1.0934999999999999</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0.71230000000000004</v>
+      </c>
+      <c r="E27" s="8">
+        <v>1.0226</v>
+      </c>
+      <c r="F27" s="8">
+        <v>2.1212</v>
+      </c>
+      <c r="G27" s="8">
+        <v>1.0321</v>
+      </c>
+      <c r="H27" s="8">
+        <v>0.46060000000000001</v>
+      </c>
+      <c r="I27" s="8">
+        <v>1.4084000000000001</v>
+      </c>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" s="8">
+        <v>1.2089000000000001</v>
+      </c>
+      <c r="C28" s="8">
+        <v>1.0224</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0.95179999999999998</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0.54769999999999996</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.47739999999999999</v>
+      </c>
+      <c r="G28" s="8">
+        <v>1.7104999999999999</v>
+      </c>
+      <c r="H28" s="8">
+        <v>2.2944</v>
+      </c>
+      <c r="I28" s="8">
+        <v>1.597</v>
+      </c>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" s="8">
+        <v>0.20430000000000001</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0.67490000000000006</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0.93289999999999995</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.58040000000000003</v>
+      </c>
+      <c r="G29" s="8">
+        <v>1.6044</v>
+      </c>
+      <c r="H29" s="8">
+        <v>1.8358000000000001</v>
+      </c>
+      <c r="I29" s="8">
+        <v>1.377</v>
+      </c>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" s="8">
+        <v>1.5696000000000001</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0.91259999999999997</v>
+      </c>
+      <c r="D30" s="8">
+        <v>0.51380000000000003</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0.69089999999999996</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.91210000000000002</v>
+      </c>
+      <c r="G30" s="8">
+        <v>1.5893999999999999</v>
+      </c>
+      <c r="H30" s="8">
+        <v>0.84570000000000001</v>
+      </c>
+      <c r="I30" s="8">
+        <v>0.6089</v>
+      </c>
+      <c r="J30" s="8"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" s="8">
+        <v>1.4593</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1.1731</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1.8857999999999999</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0.98360000000000003</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="G31" s="8">
+        <v>1.2181</v>
+      </c>
+      <c r="H31" s="8">
+        <v>2.1815000000000002</v>
+      </c>
+      <c r="I31" s="8">
+        <v>1.7170000000000001</v>
+      </c>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B32" s="8">
+        <v>1.3784000000000001</v>
+      </c>
+      <c r="C32" s="8">
+        <v>1.3018000000000001</v>
+      </c>
+      <c r="D32" s="8">
+        <v>1.5347</v>
+      </c>
+      <c r="E32" s="8">
+        <v>1.1527000000000001</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0.93149999999999999</v>
+      </c>
+      <c r="G32" s="8">
+        <v>0.91220000000000001</v>
+      </c>
+      <c r="H32" s="8">
+        <v>1.8323</v>
+      </c>
+      <c r="I32" s="8">
+        <v>1.1022000000000001</v>
+      </c>
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B33" s="8">
+        <v>1.0519000000000001</v>
+      </c>
+      <c r="C33" s="8">
+        <v>0.52090000000000003</v>
+      </c>
+      <c r="D33" s="8">
+        <v>0.85740000000000005</v>
+      </c>
+      <c r="E33" s="8">
+        <v>0.93630000000000002</v>
+      </c>
+      <c r="F33" s="8">
+        <v>1.3857999999999999</v>
+      </c>
+      <c r="G33" s="8">
+        <v>0.94730000000000003</v>
+      </c>
+      <c r="H33" s="8">
+        <v>1.6588000000000001</v>
+      </c>
+      <c r="I33" s="8">
+        <v>1.2054</v>
+      </c>
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" t="s">
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
-        <v>1</v>
-      </c>
-      <c r="H34" t="s">
-        <v>1</v>
-      </c>
-      <c r="I34" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="8">
+        <v>0.3231</v>
+      </c>
+      <c r="C34" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D34" s="8">
+        <v>2.8788</v>
+      </c>
+      <c r="E34" s="8">
+        <v>1.4278</v>
+      </c>
+      <c r="F34" s="8">
+        <v>1.4832000000000001</v>
+      </c>
+      <c r="G34" s="8">
+        <v>1.0412999999999999</v>
+      </c>
+      <c r="H34" s="8">
+        <v>1.8932</v>
+      </c>
+      <c r="I34" s="8">
+        <v>0.86809999999999998</v>
+      </c>
+      <c r="J34" s="8"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="8">
+        <v>1.1827000000000001</v>
+      </c>
+      <c r="C35" s="8">
+        <v>0.93969999999999998</v>
+      </c>
+      <c r="D35" s="8">
+        <v>1.6248</v>
+      </c>
+      <c r="E35" s="8">
+        <v>0.98680000000000001</v>
+      </c>
+      <c r="F35" s="8">
+        <v>1.1818</v>
+      </c>
+      <c r="G35" s="8">
+        <v>0.81640000000000001</v>
+      </c>
+      <c r="H35" s="8">
+        <v>1.8149999999999999</v>
+      </c>
+      <c r="I35" s="8">
+        <v>1.1063000000000001</v>
+      </c>
+      <c r="J35" s="8"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B36" s="8">
+        <v>1.74</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.75929999999999997</v>
+      </c>
+      <c r="D36" s="8">
+        <v>1.6248</v>
+      </c>
+      <c r="E36" s="8">
+        <v>1.1324000000000001</v>
+      </c>
+      <c r="F36" s="8">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="G36" s="8">
+        <v>1.679</v>
+      </c>
+      <c r="H36" s="8">
+        <v>1.3814</v>
+      </c>
+      <c r="I36" s="8">
+        <v>0.77649999999999997</v>
+      </c>
+      <c r="J36" s="8"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="8">
+        <v>1.6664000000000001</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.52280000000000004</v>
+      </c>
+      <c r="D37" s="8">
+        <v>0.84519999999999995</v>
+      </c>
+      <c r="E37" s="8">
+        <v>1.3177000000000001</v>
+      </c>
+      <c r="F37" s="8">
+        <v>2.0743</v>
+      </c>
+      <c r="G37" s="8">
+        <v>1.5098</v>
+      </c>
+      <c r="H37" s="8">
+        <v>1.3537999999999999</v>
+      </c>
+      <c r="I37" s="8">
+        <v>1.1008</v>
+      </c>
+      <c r="J37" s="8"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="8">
+        <v>1.6475</v>
+      </c>
+      <c r="C38" s="8">
+        <v>1.7133</v>
+      </c>
+      <c r="D38" s="8">
+        <v>1.7446999999999999</v>
+      </c>
+      <c r="E38" s="8">
+        <v>1.0481</v>
+      </c>
+      <c r="F38" s="8">
+        <v>1.3440000000000001</v>
+      </c>
+      <c r="G38" s="8">
+        <v>1.1195999999999999</v>
+      </c>
+      <c r="H38" s="8">
+        <v>1.2694000000000001</v>
+      </c>
+      <c r="I38" s="8">
+        <v>0.76870000000000005</v>
+      </c>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B39" s="8">
+        <v>1.042</v>
+      </c>
+      <c r="C39" s="8">
+        <v>1.5974999999999999</v>
+      </c>
+      <c r="D39" s="8">
+        <v>1.4007000000000001</v>
+      </c>
+      <c r="E39" s="8">
+        <v>1.0226</v>
+      </c>
+      <c r="F39" s="8">
+        <v>0.66469999999999996</v>
+      </c>
+      <c r="G39" s="8">
+        <v>1.3318000000000001</v>
+      </c>
+      <c r="H39" s="8">
+        <v>2.2248999999999999</v>
+      </c>
+      <c r="I39" s="8">
+        <v>1.5470999999999999</v>
+      </c>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B40" s="8">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="C40" s="8">
+        <v>0.67220000000000002</v>
+      </c>
+      <c r="D40" s="8">
+        <v>0.52869999999999995</v>
+      </c>
+      <c r="E40" s="8">
+        <v>1.2081999999999999</v>
+      </c>
+      <c r="F40" s="8">
+        <v>0.7429</v>
+      </c>
+      <c r="G40" s="8">
+        <v>0.8659</v>
+      </c>
+      <c r="H40" s="8">
+        <v>1.1871</v>
+      </c>
+      <c r="I40" s="8">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B41" s="8">
+        <v>1.8277000000000001</v>
+      </c>
+      <c r="C41" s="8">
+        <v>1.3574999999999999</v>
+      </c>
+      <c r="D41" s="8">
+        <v>1.0021</v>
+      </c>
+      <c r="E41" s="8">
+        <v>0.54190000000000005</v>
+      </c>
+      <c r="F41" s="8">
+        <v>0.63890000000000002</v>
+      </c>
+      <c r="G41" s="8">
+        <v>2.1732999999999998</v>
+      </c>
+      <c r="H41" s="8">
+        <v>2.1549999999999998</v>
+      </c>
+      <c r="I41" s="8">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="J41" s="8"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B42" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B42" s="8">
+        <v>1.7930999999999999</v>
+      </c>
+      <c r="C42" s="8">
+        <v>1.1181000000000001</v>
+      </c>
+      <c r="D42" s="8">
+        <v>1.4227000000000001</v>
+      </c>
+      <c r="E42" s="8">
+        <v>1.5443</v>
+      </c>
+      <c r="F42" s="8">
+        <v>0.72709999999999997</v>
+      </c>
+      <c r="G42" s="8">
+        <v>0.77280000000000004</v>
+      </c>
+      <c r="H42" s="8">
+        <v>1.8169</v>
+      </c>
+      <c r="I42" s="8">
+        <v>1.6092</v>
+      </c>
+      <c r="J42" s="8"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B43" s="8">
+        <v>1.042</v>
+      </c>
+      <c r="C43" s="8">
+        <v>1.0254000000000001</v>
+      </c>
+      <c r="D43" s="8">
+        <v>0.62719999999999998</v>
+      </c>
+      <c r="E43" s="8">
+        <v>0.94969999999999999</v>
+      </c>
+      <c r="F43" s="8">
+        <v>2.1854</v>
+      </c>
+      <c r="G43" s="8">
+        <v>1.9180999999999999</v>
+      </c>
+      <c r="H43" s="8">
+        <v>1.1617</v>
+      </c>
+      <c r="I43" s="8">
+        <v>1.7518</v>
+      </c>
+      <c r="J43" s="8"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B44" s="8">
+        <v>1.3708</v>
+      </c>
+      <c r="C44" s="8">
+        <v>1.3693</v>
+      </c>
+      <c r="D44" s="8">
+        <v>0.95179999999999998</v>
+      </c>
+      <c r="E44" s="8">
+        <v>0.93059999999999998</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0.3196</v>
+      </c>
+      <c r="G44" s="8">
+        <v>1.2609999999999999</v>
+      </c>
+      <c r="H44" s="8">
+        <v>0.82669999999999999</v>
+      </c>
+      <c r="I44" s="8">
+        <v>1.8489</v>
+      </c>
+      <c r="J44" s="8"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B45" s="8">
+        <v>1.1469</v>
+      </c>
+      <c r="C45" s="8">
+        <v>1.4275</v>
+      </c>
+      <c r="D45" s="8">
+        <v>0.98119999999999996</v>
+      </c>
+      <c r="E45" s="8">
+        <v>1.4504999999999999</v>
+      </c>
+      <c r="F45" s="8">
+        <v>0.23069999999999999</v>
+      </c>
+      <c r="G45" s="8">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="H45" s="8">
+        <v>0.7651</v>
+      </c>
+      <c r="I45" s="8">
+        <v>1.1659999999999999</v>
+      </c>
+      <c r="J45" s="8"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B46" s="8">
+        <v>0.91390000000000005</v>
+      </c>
+      <c r="C46" s="8">
+        <v>1.7617</v>
+      </c>
+      <c r="D46" s="8">
+        <v>1.1821999999999999</v>
+      </c>
+      <c r="E46" s="8">
+        <v>0.92379999999999995</v>
+      </c>
+      <c r="F46" s="8">
+        <v>0.34770000000000001</v>
+      </c>
+      <c r="G46" s="8">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="H46" s="8">
+        <v>2.1638000000000002</v>
+      </c>
+      <c r="I46" s="8">
+        <v>1.5056</v>
+      </c>
+      <c r="J46" s="8"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B47" s="8">
+        <v>1.7459</v>
+      </c>
+      <c r="C47" s="8">
+        <v>1.0874999999999999</v>
+      </c>
+      <c r="D47" s="8">
+        <v>0.50880000000000003</v>
+      </c>
+      <c r="E47" s="8">
+        <v>0.84619999999999995</v>
+      </c>
+      <c r="F47" s="8">
+        <v>0.53580000000000005</v>
+      </c>
+      <c r="G47" s="8">
+        <v>1.4213</v>
+      </c>
+      <c r="H47" s="8">
+        <v>1.1640999999999999</v>
+      </c>
+      <c r="I47" s="8">
+        <v>0.94620000000000004</v>
+      </c>
+      <c r="J47" s="8"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" s="8">
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="C48" s="8">
+        <v>1.0909</v>
+      </c>
+      <c r="D48" s="8">
+        <v>2.1427999999999998</v>
+      </c>
+      <c r="E48" s="8">
+        <v>0.84870000000000001</v>
+      </c>
+      <c r="F48" s="8">
+        <v>1.0019</v>
+      </c>
+      <c r="G48" s="8">
+        <v>1.1209</v>
+      </c>
+      <c r="H48" s="8">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="I48" s="8">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J48" s="8"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" s="8">
+        <v>1.8839999999999999</v>
+      </c>
+      <c r="C49" s="8">
+        <v>0.69530000000000003</v>
+      </c>
+      <c r="D49" s="8">
+        <v>2.2728999999999999</v>
+      </c>
+      <c r="E49" s="8">
+        <v>0.72230000000000005</v>
+      </c>
+      <c r="F49" s="8">
+        <v>0.91579999999999995</v>
+      </c>
+      <c r="G49" s="8">
+        <v>2.0065</v>
+      </c>
+      <c r="H49" s="8">
+        <v>1.2130000000000001</v>
+      </c>
+      <c r="I49" s="8">
+        <v>0.95569999999999999</v>
+      </c>
+      <c r="J49" s="8"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" s="8">
+        <v>0.8548</v>
+      </c>
+      <c r="C50" s="8">
+        <v>0.75239999999999996</v>
+      </c>
+      <c r="D50" s="8">
+        <v>2.5891000000000002</v>
+      </c>
+      <c r="E50" s="8">
+        <v>0.72819999999999996</v>
+      </c>
+      <c r="F50" s="8">
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="G50" s="8">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="H50" s="8">
+        <v>1.3190999999999999</v>
+      </c>
+      <c r="I50" s="8">
+        <v>1.3348</v>
+      </c>
+      <c r="J50" s="8"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" s="8">
+        <v>1.7873000000000001</v>
+      </c>
+      <c r="C51" s="8">
+        <v>0.65859999999999996</v>
+      </c>
+      <c r="D51" s="8">
+        <v>0.90439999999999998</v>
+      </c>
+      <c r="E51" s="8">
+        <v>1.2721</v>
+      </c>
+      <c r="F51" s="8">
+        <v>0.32950000000000002</v>
+      </c>
+      <c r="G51" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="H51" s="8">
+        <v>1.4088000000000001</v>
+      </c>
+      <c r="I51" s="8">
+        <v>0.73050000000000004</v>
+      </c>
+      <c r="J51" s="8"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" s="8">
+        <v>1.0618000000000001</v>
+      </c>
+      <c r="C52" s="8">
+        <v>1.1594</v>
+      </c>
+      <c r="D52" s="8">
+        <v>0.70489999999999997</v>
+      </c>
+      <c r="E52" s="8">
+        <v>1.5216000000000001</v>
+      </c>
+      <c r="F52" s="8">
+        <v>0.51139999999999997</v>
+      </c>
+      <c r="G52" s="8">
+        <v>0.64359999999999995</v>
+      </c>
+      <c r="H52" s="8">
+        <v>1.6841999999999999</v>
+      </c>
+      <c r="I52" s="8">
+        <v>1.0034000000000001</v>
+      </c>
+      <c r="J52" s="8"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" s="8">
+        <v>0.96930000000000005</v>
+      </c>
+      <c r="C53" s="8">
+        <v>0.96760000000000002</v>
+      </c>
+      <c r="D53" s="8">
+        <v>1.6812</v>
+      </c>
+      <c r="E53" s="8">
+        <v>1.0953999999999999</v>
+      </c>
+      <c r="F53" s="8">
+        <v>0.41389999999999999</v>
+      </c>
+      <c r="G53" s="8">
+        <v>1.6980999999999999</v>
+      </c>
+      <c r="H53" s="8">
+        <v>0.86060000000000003</v>
+      </c>
+      <c r="I53" s="8">
+        <v>2.0992999999999999</v>
+      </c>
+      <c r="J53" s="8"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" s="8">
+        <v>2.1528999999999998</v>
+      </c>
+      <c r="C54" s="8">
+        <v>0.91369999999999996</v>
+      </c>
+      <c r="D54" s="8">
+        <v>1.0549999999999999</v>
+      </c>
+      <c r="E54" s="8">
+        <v>0.78269999999999995</v>
+      </c>
+      <c r="F54" s="8">
+        <v>1.0494000000000001</v>
+      </c>
+      <c r="G54" s="8">
+        <v>1.0599000000000001</v>
+      </c>
+      <c r="H54" s="8">
+        <v>1.4826999999999999</v>
+      </c>
+      <c r="I54" s="8">
+        <v>1.1698999999999999</v>
+      </c>
+      <c r="J54" s="8"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" s="8">
+        <v>0.77810000000000001</v>
+      </c>
+      <c r="C55" s="8">
+        <v>0.92520000000000002</v>
+      </c>
+      <c r="D55" s="8">
+        <v>1.9278999999999999</v>
+      </c>
+      <c r="E55" s="8">
+        <v>1.2047000000000001</v>
+      </c>
+      <c r="F55" s="8">
+        <v>0.56969999999999998</v>
+      </c>
+      <c r="G55" s="8">
+        <v>0.5272</v>
+      </c>
+      <c r="H55" s="8">
+        <v>0.86409999999999998</v>
+      </c>
+      <c r="I55" s="8">
+        <v>1.4692000000000001</v>
+      </c>
+      <c r="J55" s="8"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" s="8">
+        <v>1.1099000000000001</v>
+      </c>
+      <c r="C56" s="8">
+        <v>0.68259999999999998</v>
+      </c>
+      <c r="D56" s="8">
+        <v>1.0377000000000001</v>
+      </c>
+      <c r="E56" s="8">
+        <v>0.85489999999999999</v>
+      </c>
+      <c r="F56" s="8">
+        <v>2.4138999999999999</v>
+      </c>
+      <c r="G56" s="8">
+        <v>1.4419999999999999</v>
+      </c>
+      <c r="H56" s="8">
+        <v>2.2077</v>
+      </c>
+      <c r="I56" s="8">
+        <v>1.0981000000000001</v>
+      </c>
+      <c r="J56" s="8"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" s="8">
+        <v>1.3085</v>
+      </c>
+      <c r="C57" s="8">
+        <v>0.89059999999999995</v>
+      </c>
+      <c r="D57" s="8">
+        <v>1.9835</v>
+      </c>
+      <c r="E57" s="8">
+        <v>1.3454999999999999</v>
+      </c>
+      <c r="F57" s="8">
+        <v>0.7399</v>
+      </c>
+      <c r="G57" s="8">
+        <v>1.1235999999999999</v>
+      </c>
+      <c r="H57" s="8">
+        <v>1.1217999999999999</v>
+      </c>
+      <c r="I57" s="8">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="J57" s="8"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" s="8">
+        <v>1.1738999999999999</v>
+      </c>
+      <c r="C58" s="8">
+        <v>1.5722</v>
+      </c>
+      <c r="D58" s="8">
+        <v>1.6500999999999999</v>
+      </c>
+      <c r="E58" s="8">
+        <v>1.3031999999999999</v>
+      </c>
+      <c r="F58" s="8">
+        <v>0.64810000000000001</v>
+      </c>
+      <c r="G58" s="8">
+        <v>2.5560999999999998</v>
+      </c>
+      <c r="H58" s="8">
+        <v>1.9078999999999999</v>
+      </c>
+      <c r="I58" s="8">
+        <v>1.3660000000000001</v>
+      </c>
+      <c r="J58" s="8"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" s="8">
+        <v>1.3632</v>
+      </c>
+      <c r="C59" s="8">
+        <v>1.3130999999999999</v>
+      </c>
+      <c r="D59" s="8">
+        <v>1.0276000000000001</v>
+      </c>
+      <c r="E59" s="8">
+        <v>0.8337</v>
+      </c>
+      <c r="F59" s="8">
+        <v>2.1541000000000001</v>
+      </c>
+      <c r="G59" s="8">
+        <v>0.72870000000000001</v>
+      </c>
+      <c r="H59" s="8">
+        <v>0.92610000000000003</v>
+      </c>
+      <c r="I59" s="8">
+        <v>1.0730999999999999</v>
+      </c>
+      <c r="J59" s="8"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" s="8">
+        <v>0.94750000000000001</v>
+      </c>
+      <c r="C60" s="8">
+        <v>1.2485999999999999</v>
+      </c>
+      <c r="D60" s="8">
+        <v>1.0327</v>
+      </c>
+      <c r="E60" s="8">
+        <v>1.6366000000000001</v>
+      </c>
+      <c r="F60" s="8">
+        <v>1.0434000000000001</v>
+      </c>
+      <c r="G60" s="8">
+        <v>1.1054999999999999</v>
+      </c>
+      <c r="H60" s="8">
+        <v>1.8537999999999999</v>
+      </c>
+      <c r="I60" s="8">
+        <v>1.4127000000000001</v>
+      </c>
+      <c r="J60" s="8"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" s="8">
+        <v>1.165</v>
+      </c>
+      <c r="C61" s="8">
+        <v>1.4109</v>
+      </c>
+      <c r="D61" s="8">
+        <v>2.0286</v>
+      </c>
+      <c r="E61" s="8">
+        <v>0.78269999999999995</v>
+      </c>
+      <c r="F61" s="8">
+        <v>0.62490000000000001</v>
+      </c>
+      <c r="G61" s="8">
+        <v>0.87509999999999999</v>
+      </c>
+      <c r="H61" s="8">
+        <v>2.2378</v>
+      </c>
+      <c r="I61" s="8">
+        <v>1.7892999999999999</v>
+      </c>
+      <c r="J61" s="8"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" s="8">
+        <v>1.1004</v>
+      </c>
+      <c r="C62" s="8">
+        <v>1.7112000000000001</v>
+      </c>
+      <c r="D62" s="8">
+        <v>1.3344</v>
+      </c>
+      <c r="E62" s="8">
+        <v>0.71940000000000004</v>
+      </c>
+      <c r="F62" s="8">
+        <v>0.76439999999999997</v>
+      </c>
+      <c r="G62" s="8">
+        <v>0.73409999999999997</v>
+      </c>
+      <c r="H62" s="8">
+        <v>1.59</v>
+      </c>
+      <c r="I62" s="8">
+        <v>1.3583000000000001</v>
+      </c>
+      <c r="J62" s="8"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" s="8">
+        <v>1.5427999999999999</v>
+      </c>
+      <c r="C63" s="8">
+        <v>1.2895000000000001</v>
+      </c>
+      <c r="D63" s="8">
+        <v>1.4245000000000001</v>
+      </c>
+      <c r="E63" s="8">
+        <v>1.2918000000000001</v>
+      </c>
+      <c r="F63" s="8">
+        <v>0.70960000000000001</v>
+      </c>
+      <c r="G63" s="8">
+        <v>0.86670000000000003</v>
+      </c>
+      <c r="H63" s="8">
+        <v>1.6498999999999999</v>
+      </c>
+      <c r="I63" s="8">
+        <v>1.1225000000000001</v>
+      </c>
+      <c r="J63" s="8"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" s="8">
+        <v>0.83009999999999995</v>
+      </c>
+      <c r="C64" s="8">
+        <v>0.7591</v>
+      </c>
+      <c r="D64" s="8">
+        <v>1.419</v>
+      </c>
+      <c r="E64" s="8">
+        <v>0.95309999999999995</v>
+      </c>
+      <c r="F64" s="8">
+        <v>0.2616</v>
+      </c>
+      <c r="G64" s="8">
+        <v>0.5645</v>
+      </c>
+      <c r="H64" s="8">
+        <v>0.98680000000000001</v>
+      </c>
+      <c r="I64" s="8">
+        <v>1.6958</v>
+      </c>
+      <c r="J64" s="8"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" s="8">
+        <v>0.83009999999999995</v>
+      </c>
+      <c r="C65" s="8">
+        <v>1.6618999999999999</v>
+      </c>
+      <c r="D65" s="8">
+        <v>0.63539999999999996</v>
+      </c>
+      <c r="E65" s="8">
+        <v>0.94640000000000002</v>
+      </c>
+      <c r="F65" s="8">
+        <v>0.85650000000000004</v>
+      </c>
+      <c r="G65" s="8">
+        <v>1.0501</v>
+      </c>
+      <c r="H65" s="8">
+        <v>1.0629</v>
+      </c>
+      <c r="I65" s="8">
+        <v>1.1212</v>
+      </c>
+      <c r="J65" s="8"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" s="8">
+        <v>1.1099000000000001</v>
+      </c>
+      <c r="C66" s="8">
+        <v>0.95430000000000004</v>
+      </c>
+      <c r="D66" s="8">
+        <v>1.2646999999999999</v>
+      </c>
+      <c r="E66" s="8">
+        <v>0.76770000000000005</v>
+      </c>
+      <c r="F66" s="8">
+        <v>2.0758000000000001</v>
+      </c>
+      <c r="G66" s="8">
+        <v>1.0105999999999999</v>
+      </c>
+      <c r="H66" s="8">
+        <v>2.0613000000000001</v>
+      </c>
+      <c r="I66" s="8">
+        <v>1.9442999999999999</v>
+      </c>
+      <c r="J66" s="8"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" s="8">
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="C67" s="8">
+        <v>0.51449999999999996</v>
+      </c>
+      <c r="D67" s="8">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="E67" s="8">
+        <v>1.4829000000000001</v>
+      </c>
+      <c r="F67" s="8">
+        <v>0.63839999999999997</v>
+      </c>
+      <c r="G67" s="8">
+        <v>0.97170000000000001</v>
+      </c>
+      <c r="H67" s="8">
+        <v>1.7326999999999999</v>
+      </c>
+      <c r="I67" s="8">
+        <v>0.75680000000000003</v>
+      </c>
+      <c r="J67" s="8"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" s="8">
+        <v>0.25030000000000002</v>
+      </c>
+      <c r="C68" s="8">
+        <v>1.1385000000000001</v>
+      </c>
+      <c r="D68" s="8">
+        <v>2.2269000000000001</v>
+      </c>
+      <c r="E68" s="8">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="F68" s="8">
+        <v>0.78390000000000004</v>
+      </c>
+      <c r="G68" s="8">
+        <v>0.92169999999999996</v>
+      </c>
+      <c r="H68" s="8">
+        <v>1.3149</v>
+      </c>
+      <c r="I68" s="8">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="J68" s="8"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <f t="shared" ref="A69" si="1">A68+1</f>
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" s="8">
+        <v>1.7930999999999999</v>
+      </c>
+      <c r="C69" s="8">
+        <v>1.6087</v>
+      </c>
+      <c r="D69" s="8">
+        <v>2.0274000000000001</v>
+      </c>
+      <c r="E69" s="8">
+        <v>1.4498</v>
+      </c>
+      <c r="F69" s="8">
+        <v>0.77829999999999999</v>
+      </c>
+      <c r="G69" s="8">
+        <v>1.2975000000000001</v>
+      </c>
+      <c r="H69" s="8">
+        <v>1.1884999999999999</v>
+      </c>
+      <c r="I69" s="8">
+        <v>1.0730999999999999</v>
+      </c>
+      <c r="J69" s="8"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" s="8">
+        <v>2.1432000000000002</v>
+      </c>
+      <c r="C70" s="8">
+        <v>1.1026</v>
+      </c>
+      <c r="D70" s="8">
+        <v>0.61470000000000002</v>
+      </c>
+      <c r="E70" s="8">
+        <v>1.1453</v>
+      </c>
+      <c r="F70" s="8">
+        <v>0.73350000000000004</v>
+      </c>
+      <c r="G70" s="8">
+        <v>0.76680000000000004</v>
+      </c>
+      <c r="H70" s="8">
+        <v>1.8514999999999999</v>
+      </c>
+      <c r="I70" s="8">
+        <v>1.3062</v>
+      </c>
+      <c r="J70" s="8"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <f t="shared" ref="A71:A102" si="2">A70+1</f>
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" s="8">
+        <v>0.87890000000000001</v>
+      </c>
+      <c r="C71" s="8">
+        <v>1.6775</v>
+      </c>
+      <c r="D71" s="8">
+        <v>0.99170000000000003</v>
+      </c>
+      <c r="E71" s="8">
+        <v>1.2063999999999999</v>
+      </c>
+      <c r="F71" s="8">
+        <v>1.2441</v>
+      </c>
+      <c r="G71" s="8">
+        <v>1.8056000000000001</v>
+      </c>
+      <c r="H71" s="8">
+        <v>1.7124999999999999</v>
+      </c>
+      <c r="I71" s="8">
+        <v>1.4338</v>
+      </c>
+      <c r="J71" s="8"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" s="8">
+        <v>0.93640000000000001</v>
+      </c>
+      <c r="C72" s="8">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="D72" s="8">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="E72" s="8">
+        <v>1.4807999999999999</v>
+      </c>
+      <c r="F72" s="8">
+        <v>0.31290000000000001</v>
+      </c>
+      <c r="G72" s="8">
+        <v>0.80379999999999996</v>
+      </c>
+      <c r="H72" s="8">
+        <v>0.98480000000000001</v>
+      </c>
+      <c r="I72" s="8">
+        <v>1.2447999999999999</v>
+      </c>
+      <c r="J72" s="8"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" s="8">
+        <v>1.2261</v>
+      </c>
+      <c r="C73" s="8">
+        <v>0.94140000000000001</v>
+      </c>
+      <c r="D73" s="8">
+        <v>1.8968</v>
+      </c>
+      <c r="E73" s="8">
+        <v>1.5382</v>
+      </c>
+      <c r="F73" s="8">
+        <v>0.78410000000000002</v>
+      </c>
+      <c r="G73" s="8">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="H73" s="8">
+        <v>1.0639000000000001</v>
+      </c>
+      <c r="I73" s="8">
+        <v>1.9947999999999999</v>
+      </c>
+      <c r="J73" s="8"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <f t="shared" si="2"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" s="8">
+        <v>2.0177999999999998</v>
+      </c>
+      <c r="C74" s="8">
+        <v>0.83779999999999999</v>
+      </c>
+      <c r="D74" s="8">
+        <v>1.2358</v>
+      </c>
+      <c r="E74" s="8">
+        <v>0.75939999999999996</v>
+      </c>
+      <c r="F74" s="8">
+        <v>0.88349999999999995</v>
+      </c>
+      <c r="G74" s="8">
+        <v>1.1677999999999999</v>
+      </c>
+      <c r="H74" s="8">
+        <v>2.0103</v>
+      </c>
+      <c r="I74" s="8">
+        <v>1.7518</v>
+      </c>
+      <c r="J74" s="8"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <f t="shared" si="2"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" s="8">
+        <v>1.4157999999999999</v>
+      </c>
+      <c r="C75" s="8">
+        <v>1.0418000000000001</v>
+      </c>
+      <c r="D75" s="8">
+        <v>0.6633</v>
+      </c>
+      <c r="E75" s="8">
+        <v>0.75660000000000005</v>
+      </c>
+      <c r="F75" s="8">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="G75" s="8">
+        <v>1.9630000000000001</v>
+      </c>
+      <c r="H75" s="8">
+        <v>1.2316</v>
+      </c>
+      <c r="I75" s="8">
+        <v>0.89880000000000004</v>
+      </c>
+      <c r="J75" s="8"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <f t="shared" si="2"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" s="8">
+        <v>1.0519000000000001</v>
+      </c>
+      <c r="C76" s="8">
+        <v>0.86119999999999997</v>
+      </c>
+      <c r="D76" s="8">
+        <v>2.3147000000000002</v>
+      </c>
+      <c r="E76" s="8">
+        <v>1.0027999999999999</v>
+      </c>
+      <c r="F76" s="8">
+        <v>0.72770000000000001</v>
+      </c>
+      <c r="G76" s="8">
+        <v>0.81210000000000004</v>
+      </c>
+      <c r="H76" s="8">
+        <v>1.8028</v>
+      </c>
+      <c r="I76" s="8">
+        <v>1.1049</v>
+      </c>
+      <c r="J76" s="8"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" s="8">
+        <v>1.0618000000000001</v>
+      </c>
+      <c r="C77" s="8">
+        <v>1.1618999999999999</v>
+      </c>
+      <c r="D77" s="8">
+        <v>1.6008</v>
+      </c>
+      <c r="E77" s="8">
+        <v>1.3493999999999999</v>
+      </c>
+      <c r="F77" s="8">
+        <v>0.67910000000000004</v>
+      </c>
+      <c r="G77" s="8">
+        <v>1.0085999999999999</v>
+      </c>
+      <c r="H77" s="8">
+        <v>0.64580000000000004</v>
+      </c>
+      <c r="I77" s="8">
+        <v>0.74070000000000003</v>
+      </c>
+      <c r="J77" s="8"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" s="8">
+        <v>1.34</v>
+      </c>
+      <c r="C78" s="8">
+        <v>0.81510000000000005</v>
+      </c>
+      <c r="D78" s="8">
+        <v>1.528</v>
+      </c>
+      <c r="E78" s="8">
+        <v>1.2238</v>
+      </c>
+      <c r="F78" s="8">
+        <v>2.1989000000000001</v>
+      </c>
+      <c r="G78" s="8">
+        <v>0.68689999999999996</v>
+      </c>
+      <c r="H78" s="8">
+        <v>0.87960000000000005</v>
+      </c>
+      <c r="I78" s="8">
+        <v>1.6717</v>
+      </c>
+      <c r="J78" s="8"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" s="8">
+        <v>1.4877</v>
+      </c>
+      <c r="C79" s="8">
+        <v>0.54369999999999996</v>
+      </c>
+      <c r="D79" s="8">
+        <v>1.6485000000000001</v>
+      </c>
+      <c r="E79" s="8">
+        <v>0.42370000000000002</v>
+      </c>
+      <c r="F79" s="8">
+        <v>0.67920000000000003</v>
+      </c>
+      <c r="G79" s="8">
+        <v>1.5545</v>
+      </c>
+      <c r="H79" s="8">
+        <v>2.3206000000000002</v>
+      </c>
+      <c r="I79" s="8">
+        <v>1.403</v>
+      </c>
+      <c r="J79" s="8"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <f t="shared" si="2"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" s="8">
+        <v>1.4593</v>
+      </c>
+      <c r="C80" s="8">
+        <v>1.4591000000000001</v>
+      </c>
+      <c r="D80" s="8">
+        <v>1.8413999999999999</v>
+      </c>
+      <c r="E80" s="8">
+        <v>1.4337</v>
+      </c>
+      <c r="F80" s="8">
+        <v>0.61229999999999996</v>
+      </c>
+      <c r="G80" s="8">
+        <v>0.71579999999999999</v>
+      </c>
+      <c r="H80" s="8">
+        <v>0.44269999999999998</v>
+      </c>
+      <c r="I80" s="8">
+        <v>0.74880000000000002</v>
+      </c>
+      <c r="J80" s="8"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" s="8">
+        <v>0.14449999999999999</v>
+      </c>
+      <c r="C81" s="8">
+        <v>0.5776</v>
+      </c>
+      <c r="D81" s="8">
+        <v>1.8913</v>
+      </c>
+      <c r="E81" s="8">
+        <v>1.4292</v>
+      </c>
+      <c r="F81" s="8">
+        <v>2.5568</v>
+      </c>
+      <c r="G81" s="8">
+        <v>0.89270000000000005</v>
+      </c>
+      <c r="H81" s="8">
+        <v>1.2351000000000001</v>
+      </c>
+      <c r="I81" s="8">
+        <v>1.2253000000000001</v>
+      </c>
+      <c r="J81" s="8"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" s="8">
+        <v>0.76459999999999995</v>
+      </c>
+      <c r="C82" s="8">
+        <v>0.95040000000000002</v>
+      </c>
+      <c r="D82" s="8">
+        <v>2.1511999999999998</v>
+      </c>
+      <c r="E82" s="8">
+        <v>1.0953999999999999</v>
+      </c>
+      <c r="F82" s="8">
+        <v>1.4273</v>
+      </c>
+      <c r="G82" s="8">
+        <v>1.5062</v>
+      </c>
+      <c r="H82" s="8">
+        <v>2.1192000000000002</v>
+      </c>
+      <c r="I82" s="8">
+        <v>0.76870000000000005</v>
+      </c>
+      <c r="J82" s="8"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" s="8">
+        <v>1.4009</v>
+      </c>
+      <c r="C83" s="8">
+        <v>1.0585</v>
+      </c>
+      <c r="D83" s="8">
+        <v>0.41949999999999998</v>
+      </c>
+      <c r="E83" s="8">
+        <v>1.4943</v>
+      </c>
+      <c r="F83" s="8">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="G83" s="8">
+        <v>1.6835</v>
+      </c>
+      <c r="H83" s="8">
+        <v>1.7801</v>
+      </c>
+      <c r="I83" s="8">
+        <v>0.81069999999999998</v>
+      </c>
+      <c r="J83" s="8"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <f t="shared" si="2"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" s="8">
+        <v>0.4335</v>
+      </c>
+      <c r="C84" s="8">
+        <v>1.6607000000000001</v>
+      </c>
+      <c r="D84" s="8">
+        <v>1.4336</v>
+      </c>
+      <c r="E84" s="8">
+        <v>0.92149999999999999</v>
+      </c>
+      <c r="F84" s="8">
+        <v>1.4901</v>
+      </c>
+      <c r="G84" s="8">
+        <v>1.1143000000000001</v>
+      </c>
+      <c r="H84" s="8">
+        <v>0.73370000000000002</v>
+      </c>
+      <c r="I84" s="8">
+        <v>1.1008</v>
+      </c>
+      <c r="J84" s="8"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <f t="shared" si="2"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" s="8">
+        <v>1.4084000000000001</v>
+      </c>
+      <c r="C85" s="8">
+        <v>1.3729</v>
+      </c>
+      <c r="D85" s="8">
+        <v>0.51880000000000004</v>
+      </c>
+      <c r="E85" s="8">
+        <v>1.0226</v>
+      </c>
+      <c r="F85" s="8">
+        <v>0.68110000000000004</v>
+      </c>
+      <c r="G85" s="8">
+        <v>1.7964</v>
+      </c>
+      <c r="H85" s="8">
+        <v>0.56889999999999996</v>
+      </c>
+      <c r="I85" s="8">
+        <v>0.92530000000000001</v>
+      </c>
+      <c r="J85" s="8"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <f t="shared" si="2"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" s="8">
+        <v>1.8504</v>
+      </c>
+      <c r="C86" s="8">
+        <v>0.64949999999999997</v>
+      </c>
+      <c r="D86" s="8">
+        <v>0.50360000000000005</v>
+      </c>
+      <c r="E86" s="8">
+        <v>1.2255</v>
+      </c>
+      <c r="F86" s="8">
+        <v>2.3576000000000001</v>
+      </c>
+      <c r="G86" s="8">
+        <v>1.2643</v>
+      </c>
+      <c r="H86" s="8">
+        <v>2.2433000000000001</v>
+      </c>
+      <c r="I86" s="8">
+        <v>1.4712000000000001</v>
+      </c>
+      <c r="J86" s="8"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <f t="shared" si="2"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" s="8">
+        <v>0.73680000000000001</v>
+      </c>
+      <c r="C87" s="8">
+        <v>0.90390000000000004</v>
+      </c>
+      <c r="D87" s="8">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="E87" s="8">
+        <v>1.0174000000000001</v>
+      </c>
+      <c r="F87" s="8">
+        <v>0.96809999999999996</v>
+      </c>
+      <c r="G87" s="8">
+        <v>1.0811999999999999</v>
+      </c>
+      <c r="H87" s="8">
+        <v>1.4429000000000001</v>
+      </c>
+      <c r="I87" s="8">
+        <v>1.0646</v>
+      </c>
+      <c r="J87" s="8"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <f t="shared" si="2"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88" s="8">
+        <v>1.5495000000000001</v>
+      </c>
+      <c r="C88" s="8">
+        <v>1.083</v>
+      </c>
+      <c r="D88" s="8">
+        <v>1.7461</v>
+      </c>
+      <c r="E88" s="8">
+        <v>0.84870000000000001</v>
+      </c>
+      <c r="F88" s="8">
+        <v>0.70379999999999998</v>
+      </c>
+      <c r="G88" s="8">
+        <v>0.91239999999999999</v>
+      </c>
+      <c r="H88" s="8">
+        <v>1.5485</v>
+      </c>
+      <c r="I88" s="8">
+        <v>1.3527</v>
+      </c>
+      <c r="J88" s="8"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <f t="shared" si="2"/>
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" s="8">
+        <v>0.5958</v>
+      </c>
+      <c r="C89" s="8">
+        <v>1.4923</v>
+      </c>
+      <c r="D89" s="8">
+        <v>1.9144000000000001</v>
+      </c>
+      <c r="E89" s="8">
+        <v>0.93179999999999996</v>
+      </c>
+      <c r="F89" s="8">
+        <v>1.1701999999999999</v>
+      </c>
+      <c r="G89" s="8">
+        <v>1.3302</v>
+      </c>
+      <c r="H89" s="8">
+        <v>0.88590000000000002</v>
+      </c>
+      <c r="I89" s="8">
+        <v>1.0345</v>
+      </c>
+      <c r="J89" s="8"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <f t="shared" si="2"/>
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" s="8">
+        <v>1.5696000000000001</v>
+      </c>
+      <c r="C90" s="8">
+        <v>1.5290999999999999</v>
+      </c>
+      <c r="D90" s="8">
+        <v>3.0979999999999999</v>
+      </c>
+      <c r="E90" s="8">
+        <v>1.1888000000000001</v>
+      </c>
+      <c r="F90" s="8">
+        <v>0.50170000000000003</v>
+      </c>
+      <c r="G90" s="8">
+        <v>1.3293999999999999</v>
+      </c>
+      <c r="H90" s="8">
+        <v>1.7150000000000001</v>
+      </c>
+      <c r="I90" s="8">
+        <v>0.72419999999999995</v>
+      </c>
+      <c r="J90" s="8"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <f t="shared" si="2"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" s="8">
+        <v>1.1004</v>
+      </c>
+      <c r="C91" s="8">
+        <v>1.2717000000000001</v>
+      </c>
+      <c r="D91" s="8">
+        <v>2.3191999999999999</v>
+      </c>
+      <c r="E91" s="8">
+        <v>1.1378999999999999</v>
+      </c>
+      <c r="F91" s="8">
+        <v>1.5898000000000001</v>
+      </c>
+      <c r="G91" s="8">
+        <v>0.66579999999999995</v>
+      </c>
+      <c r="H91" s="8">
+        <v>0.71819999999999995</v>
+      </c>
+      <c r="I91" s="8">
+        <v>0.91210000000000002</v>
+      </c>
+      <c r="J91" s="8"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" s="8">
+        <v>1.5495000000000001</v>
+      </c>
+      <c r="C92" s="8">
+        <v>0.72289999999999999</v>
+      </c>
+      <c r="D92" s="8">
+        <v>0.50880000000000003</v>
+      </c>
+      <c r="E92" s="8">
+        <v>0.83240000000000003</v>
+      </c>
+      <c r="F92" s="8">
+        <v>0.6704</v>
+      </c>
+      <c r="G92" s="8">
+        <v>1.2855000000000001</v>
+      </c>
+      <c r="H92" s="8">
+        <v>2.2061000000000002</v>
+      </c>
+      <c r="I92" s="8">
+        <v>0.73660000000000003</v>
+      </c>
+      <c r="J92" s="8"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" s="8">
+        <v>2.1528999999999998</v>
+      </c>
+      <c r="C93" s="8">
+        <v>1.5406</v>
+      </c>
+      <c r="D93" s="8">
+        <v>2.0055000000000001</v>
+      </c>
+      <c r="E93" s="8">
+        <v>0.70760000000000001</v>
+      </c>
+      <c r="F93" s="8">
+        <v>1.3660000000000001</v>
+      </c>
+      <c r="G93" s="8">
+        <v>1.0530999999999999</v>
+      </c>
+      <c r="H93" s="8">
+        <v>1.5521</v>
+      </c>
+      <c r="I93" s="8">
+        <v>1.8250999999999999</v>
+      </c>
+      <c r="J93" s="8"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <f t="shared" si="2"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" s="8">
+        <v>1.0618000000000001</v>
+      </c>
+      <c r="C94" s="8">
+        <v>1.3062</v>
+      </c>
+      <c r="D94" s="8">
+        <v>1.3593999999999999</v>
+      </c>
+      <c r="E94" s="8">
+        <v>1.2737000000000001</v>
+      </c>
+      <c r="F94" s="8">
+        <v>0.79569999999999996</v>
+      </c>
+      <c r="G94" s="8">
+        <v>0.88870000000000005</v>
+      </c>
+      <c r="H94" s="8">
+        <v>1.5024999999999999</v>
+      </c>
+      <c r="I94" s="8">
+        <v>1.2079</v>
+      </c>
+      <c r="J94" s="8"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <f t="shared" si="2"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" s="8">
+        <v>1.609</v>
+      </c>
+      <c r="C95" s="8">
+        <v>0.72130000000000005</v>
+      </c>
+      <c r="D95" s="8">
+        <v>1.0768</v>
+      </c>
+      <c r="E95" s="8">
+        <v>1.1002000000000001</v>
+      </c>
+      <c r="F95" s="8">
+        <v>0.60489999999999999</v>
+      </c>
+      <c r="G95" s="8">
+        <v>1.2965</v>
+      </c>
+      <c r="H95" s="8">
+        <v>0.71360000000000001</v>
+      </c>
+      <c r="I95" s="8">
+        <v>1.0518000000000001</v>
+      </c>
+      <c r="J95" s="8"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <f t="shared" si="2"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B96" s="8">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="C96" s="8">
+        <v>0.54149999999999998</v>
+      </c>
+      <c r="D96" s="8">
+        <v>0.80759999999999998</v>
+      </c>
+      <c r="E96" s="8">
+        <v>1.0122</v>
+      </c>
+      <c r="F96" s="8">
+        <v>1.0851</v>
+      </c>
+      <c r="G96" s="8">
+        <v>1.4378</v>
+      </c>
+      <c r="H96" s="8">
+        <v>1.8835</v>
+      </c>
+      <c r="I96" s="8">
+        <v>1.0857000000000001</v>
+      </c>
+      <c r="J96" s="8"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <f t="shared" si="2"/>
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B97" s="8">
+        <v>1.0812999999999999</v>
+      </c>
+      <c r="C97" s="8">
+        <v>0.93079999999999996</v>
+      </c>
+      <c r="D97" s="8">
+        <v>2.3313999999999999</v>
+      </c>
+      <c r="E97" s="8">
+        <v>1.0348999999999999</v>
+      </c>
+      <c r="F97" s="8">
+        <v>0.39850000000000002</v>
+      </c>
+      <c r="G97" s="8">
+        <v>2.1465999999999998</v>
+      </c>
+      <c r="H97" s="8">
+        <v>1.2882</v>
+      </c>
+      <c r="I97" s="8">
+        <v>0.88019999999999998</v>
+      </c>
+      <c r="J97" s="8"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B98" s="8">
+        <v>1.042</v>
+      </c>
+      <c r="C98" s="8">
+        <v>0.92210000000000003</v>
+      </c>
+      <c r="D98" s="8">
+        <v>2.1869999999999998</v>
+      </c>
+      <c r="E98" s="8">
+        <v>1.1088</v>
+      </c>
+      <c r="F98" s="8">
+        <v>0.83709999999999996</v>
+      </c>
+      <c r="G98" s="8">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="H98" s="8">
+        <v>1.7717000000000001</v>
+      </c>
+      <c r="I98" s="8">
+        <v>1.0048999999999999</v>
+      </c>
+      <c r="J98" s="8"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B99" s="8">
+        <v>1.1285000000000001</v>
+      </c>
+      <c r="C99" s="8">
+        <v>0.57310000000000005</v>
+      </c>
+      <c r="D99" s="8">
+        <v>1.6827000000000001</v>
+      </c>
+      <c r="E99" s="8">
+        <v>0.97709999999999997</v>
+      </c>
+      <c r="F99" s="8">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="G99" s="8">
+        <v>1.7291000000000001</v>
+      </c>
+      <c r="H99" s="8">
+        <v>1.4569000000000001</v>
+      </c>
+      <c r="I99" s="8">
+        <v>1.2202999999999999</v>
+      </c>
+      <c r="J99" s="8"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <f t="shared" si="2"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B100" s="8">
+        <v>2.0689000000000002</v>
+      </c>
+      <c r="C100" s="8">
+        <v>1.2490000000000001</v>
+      </c>
+      <c r="D100" s="8">
+        <v>0.83909999999999996</v>
+      </c>
+      <c r="E100" s="8">
+        <v>0.95860000000000001</v>
+      </c>
+      <c r="F100" s="8">
+        <v>0.61909999999999998</v>
+      </c>
+      <c r="G100" s="8">
+        <v>1.1782999999999999</v>
+      </c>
+      <c r="H100" s="8">
+        <v>1.2432000000000001</v>
+      </c>
+      <c r="I100" s="8">
+        <v>1.5116000000000001</v>
+      </c>
+      <c r="J100" s="8"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <f t="shared" si="2"/>
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B101" s="8">
+        <v>2.177</v>
+      </c>
+      <c r="C101" s="8">
+        <v>0.82620000000000005</v>
+      </c>
+      <c r="D101" s="8">
+        <v>3.5371999999999999</v>
+      </c>
+      <c r="E101" s="8">
+        <v>1.0389999999999999</v>
+      </c>
+      <c r="F101" s="8">
+        <v>0.65859999999999996</v>
+      </c>
+      <c r="G101" s="8">
+        <v>1.9549000000000001</v>
+      </c>
+      <c r="H101" s="8">
+        <v>1.42</v>
+      </c>
+      <c r="I101" s="8">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="J101" s="8"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B102" s="8">
+        <v>0.87890000000000001</v>
+      </c>
+      <c r="C102" s="8">
+        <v>0.5423</v>
+      </c>
+      <c r="D102" s="8">
+        <v>3.0568</v>
+      </c>
+      <c r="E102" s="8">
+        <v>0.65810000000000002</v>
+      </c>
+      <c r="F102" s="8">
+        <v>0.88190000000000002</v>
+      </c>
+      <c r="G102" s="8">
+        <v>1.3925000000000001</v>
+      </c>
+      <c r="H102" s="8">
+        <v>1.9827999999999999</v>
+      </c>
+      <c r="I102" s="8">
+        <v>0.8236</v>
+      </c>
+      <c r="J102" s="8"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B103" s="8"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="8"/>
+      <c r="G103" s="8"/>
+      <c r="H103" s="8"/>
+      <c r="I103" s="8"/>
+      <c r="J103" s="8"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B104" s="6">
         <f>SUM(B3:B102)/100</f>
-        <v>0</v>
+        <v>1.224685</v>
       </c>
       <c r="C104" s="6">
         <f t="shared" ref="C104:I104" si="3">SUM(C3:C102)/100</f>
-        <v>0</v>
+        <v>1.0475639999999997</v>
       </c>
       <c r="D104" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.4604670000000006</v>
       </c>
       <c r="E104" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.0549249999999994</v>
       </c>
       <c r="F104" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.98893900000000012</v>
       </c>
       <c r="G104" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.2037880000000001</v>
       </c>
       <c r="H104" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.4963599999999999</v>
       </c>
       <c r="I104" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.228971</v>
       </c>
     </row>
   </sheetData>

</xml_diff>